<commit_message>
updating snap model for Q1'24.
</commit_message>
<xml_diff>
--- a/SNAP.xlsx
+++ b/SNAP.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameelbrannon/Library/CloudStorage/Dropbox/Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E1F47F-74D8-F24D-AF33-819DC7FE4695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C370A2-6A57-D44A-94A7-146AD92E3B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8680" yWindow="600" windowWidth="40280" windowHeight="27160" xr2:uid="{0631FB18-10CE-5B46-8C21-F517C35CE685}"/>
+    <workbookView xWindow="25780" yWindow="500" windowWidth="26860" windowHeight="27160" activeTab="1" xr2:uid="{0631FB18-10CE-5B46-8C21-F517C35CE685}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Model" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.1" hidden="1">Model!$C$13:$N$13</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">Model!$C$13:$N$13</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,8 +36,27 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={8423C853-32E6-F247-9D6B-FB819A2D6B15}</author>
+  </authors>
+  <commentList>
+    <comment ref="P6" authorId="0" shapeId="0" xr:uid="{8423C853-32E6-F247-9D6B-FB819A2D6B15}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    GUIDANCE
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="83">
   <si>
     <t>P</t>
   </si>
@@ -278,6 +293,18 @@
   </si>
   <si>
     <t>Evan Spiegel</t>
+  </si>
+  <si>
+    <t>4Q FCF</t>
+  </si>
+  <si>
+    <t>4Q NI</t>
+  </si>
+  <si>
+    <t>Q1'24</t>
+  </si>
+  <si>
+    <t>PRESSES</t>
   </si>
 </sst>
 </file>
@@ -285,9 +312,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.000000\x"/>
+    <numFmt numFmtId="164" formatCode="0.000000\x"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -314,6 +341,17 @@
       <name val="ArialMT"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="ArialMT"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -336,7 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -347,8 +385,11 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -371,16 +412,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>15554</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>81642</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>15555</xdr:colOff>
       <xdr:row>82</xdr:row>
-      <xdr:rowOff>117928</xdr:rowOff>
+      <xdr:rowOff>36286</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -395,8 +436,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6268357" y="81642"/>
-          <a:ext cx="1" cy="13262429"/>
+          <a:off x="7491621" y="0"/>
+          <a:ext cx="1" cy="13921619"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -472,6 +513,12 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="jameel" id="{CF8E9CCF-14E4-7E46-B16E-40A862A5834E}" userId="jameel" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -769,12 +816,21 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="P6" dT="2024-05-13T02:54:57.55" personId="{CF8E9CCF-14E4-7E46-B16E-40A862A5834E}" id="{8423C853-32E6-F247-9D6B-FB819A2D6B15}">
+    <text xml:space="preserve">GUIDANCE
+</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157A76BE-B473-3F48-9E48-C63C96553EE5}">
   <dimension ref="B2:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="279" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView zoomScale="279" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -806,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="3">
-        <v>11.14</v>
+        <v>16.010000000000002</v>
       </c>
     </row>
     <row r="5" spans="2:10">
@@ -814,11 +870,11 @@
         <v>1</v>
       </c>
       <c r="G5" s="1">
-        <f>1396.476171+22.528406+231.626943</f>
-        <v>1650.6315199999999</v>
+        <f>1386.883641+22.528406+231.626943</f>
+        <v>1641.0389899999998</v>
       </c>
       <c r="H5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:10">
@@ -827,32 +883,38 @@
       </c>
       <c r="G6" s="1">
         <f>+G4*G5</f>
-        <v>18388.0351328</v>
+        <v>26273.0342299</v>
       </c>
     </row>
     <row r="7" spans="2:10">
+      <c r="C7" s="14" t="s">
+        <v>82</v>
+      </c>
       <c r="F7" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="1">
-        <f>1780.4+1763.68</f>
-        <v>3544.08</v>
+        <f>1060.393+1850.622</f>
+        <v>2911.0150000000003</v>
       </c>
       <c r="H7" t="str">
         <f>+H5</f>
-        <v>Q423</v>
+        <v>Q124</v>
       </c>
     </row>
     <row r="8" spans="2:10">
+      <c r="C8" s="13" t="s">
+        <v>81</v>
+      </c>
       <c r="F8" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="1">
-        <v>3749.4</v>
+        <v>3301.4659999999999</v>
       </c>
       <c r="H8" t="str">
         <f>+H7</f>
-        <v>Q423</v>
+        <v>Q124</v>
       </c>
     </row>
     <row r="9" spans="2:10">
@@ -861,34 +923,37 @@
       </c>
       <c r="G9" s="1">
         <f>+G6-G7+G8</f>
-        <v>18593.355132799999</v>
+        <v>26663.485229900001</v>
       </c>
       <c r="J9" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C8" r:id="rId1" xr:uid="{C9A628C5-3623-7046-BC99-8C2159468C0F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6F94D9-2E34-0746-A768-A741782B4BA6}">
-  <dimension ref="A1:AQ73"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6F94D9-2E34-0746-A768-A741782B4BA6}">
+  <dimension ref="A1:AQ76"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AT33" sqref="AT33"/>
+      <selection pane="bottomRight" activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="4.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="12" width="5.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.83203125" style="1" customWidth="1"/>
-    <col min="15" max="18" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="14" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="5.5" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="22" width="5.5" style="1" customWidth="1"/>
     <col min="23" max="23" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
@@ -1064,6 +1129,9 @@
       <c r="N3" s="2">
         <v>100</v>
       </c>
+      <c r="O3" s="2">
+        <v>100</v>
+      </c>
       <c r="AB3" s="2">
         <f>+J3</f>
         <v>100</v>
@@ -1113,6 +1181,9 @@
       <c r="N4" s="2">
         <v>96</v>
       </c>
+      <c r="O4" s="2">
+        <v>96</v>
+      </c>
       <c r="AB4" s="2">
         <f t="shared" ref="AB4:AB6" si="1">+J4</f>
         <v>92</v>
@@ -1162,6 +1233,9 @@
       <c r="N5" s="2">
         <v>218</v>
       </c>
+      <c r="O5" s="2">
+        <v>226</v>
+      </c>
       <c r="AB5" s="2">
         <f t="shared" si="1"/>
         <v>183</v>
@@ -1192,7 +1266,7 @@
         <v>319</v>
       </c>
       <c r="G6" s="5">
-        <f t="shared" ref="G6:N6" si="4">SUM(G3:G5)</f>
+        <f t="shared" ref="G6:O6" si="4">SUM(G3:G5)</f>
         <v>332</v>
       </c>
       <c r="H6" s="5">
@@ -1224,19 +1298,19 @@
         <v>414</v>
       </c>
       <c r="O6" s="5">
-        <v>420</v>
+        <f t="shared" si="4"/>
+        <v>422</v>
       </c>
       <c r="P6" s="5">
-        <f>+O6+6</f>
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="Q6" s="5">
         <f>+P6+6</f>
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="R6" s="5">
         <f>+Q6+6</f>
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="AB6" s="2">
         <f t="shared" si="1"/>
@@ -1248,43 +1322,43 @@
       </c>
       <c r="AD6" s="5">
         <f>+R6</f>
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="AE6" s="5">
         <f>+AD6+20</f>
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="AF6" s="5">
         <f t="shared" ref="AF6:AM6" si="5">+AE6+20</f>
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="AG6" s="5">
         <f t="shared" si="5"/>
-        <v>498</v>
+        <v>503</v>
       </c>
       <c r="AH6" s="5">
         <f t="shared" si="5"/>
-        <v>518</v>
+        <v>523</v>
       </c>
       <c r="AI6" s="5">
         <f t="shared" si="5"/>
-        <v>538</v>
+        <v>543</v>
       </c>
       <c r="AJ6" s="5">
         <f t="shared" si="5"/>
-        <v>558</v>
+        <v>563</v>
       </c>
       <c r="AK6" s="5">
         <f t="shared" si="5"/>
-        <v>578</v>
+        <v>583</v>
       </c>
       <c r="AL6" s="5">
         <f t="shared" si="5"/>
-        <v>598</v>
+        <v>603</v>
       </c>
       <c r="AM6" s="5">
         <f t="shared" si="5"/>
-        <v>618</v>
+        <v>623</v>
       </c>
     </row>
     <row r="7" spans="1:39" s="2" customFormat="1">
@@ -1371,19 +1445,19 @@
       </c>
       <c r="O8" s="6">
         <f>+O13/O6</f>
-        <v>2.6547619047619047</v>
+        <v>2.8312156398104262</v>
       </c>
       <c r="P8" s="6">
         <f>+O8*1.05</f>
-        <v>2.7875000000000001</v>
+        <v>2.9727764218009476</v>
       </c>
       <c r="Q8" s="6">
         <f>+P8*1.05</f>
-        <v>2.9268750000000003</v>
+        <v>3.1214152428909951</v>
       </c>
       <c r="R8" s="6">
         <f>+Q8*1.05</f>
-        <v>3.0732187500000006</v>
+        <v>3.277486005035545</v>
       </c>
       <c r="AB8" s="6">
         <f t="shared" ref="AB8:AC8" si="9">+IFERROR(AB13/AB6,0)</f>
@@ -1476,7 +1550,44 @@
       </c>
     </row>
     <row r="10" spans="1:39" s="2" customFormat="1"/>
-    <row r="11" spans="1:39" s="2" customFormat="1"/>
+    <row r="11" spans="1:39" s="2" customFormat="1">
+      <c r="G11" s="7">
+        <f t="shared" ref="G11:N11" si="11">+G8/C8-1</f>
+        <v>0.16878309329753383</v>
+      </c>
+      <c r="H11" s="7">
+        <f t="shared" si="11"/>
+        <v>-0.15561959654178681</v>
+      </c>
+      <c r="I11" s="7">
+        <f t="shared" si="11"/>
+        <v>-0.10884952447776253</v>
+      </c>
+      <c r="J11" s="7">
+        <f t="shared" si="11"/>
+        <v>-0.14812079652665677</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" si="11"/>
+        <v>-0.19361634600218036</v>
+      </c>
+      <c r="L11" s="7">
+        <f t="shared" si="11"/>
+        <v>-0.15996551334400577</v>
+      </c>
+      <c r="M11" s="7">
+        <f t="shared" si="11"/>
+        <v>-6.0627784729139211E-2</v>
+      </c>
+      <c r="N11" s="7">
+        <f t="shared" si="11"/>
+        <v>-5.1306751883591795E-2</v>
+      </c>
+      <c r="O11" s="7">
+        <f>+O8/K8-1</f>
+        <v>9.6850915678806215E-2</v>
+      </c>
+    </row>
     <row r="12" spans="1:39" s="2" customFormat="1"/>
     <row r="13" spans="1:39">
       <c r="B13" s="1" t="s">
@@ -1519,20 +1630,19 @@
         <v>1361.287</v>
       </c>
       <c r="O13" s="1">
-        <f>AVERAGE(1095,1135)</f>
-        <v>1115</v>
+        <v>1194.7729999999999</v>
       </c>
       <c r="P13" s="1">
         <f>+P6*P8</f>
-        <v>1187.4750000000001</v>
+        <v>1281.2666377962084</v>
       </c>
       <c r="Q13" s="1">
         <f>+Q6*Q8</f>
-        <v>1264.4100000000001</v>
+        <v>1364.0584611433649</v>
       </c>
       <c r="R13" s="1">
         <f>+R6*R8</f>
-        <v>1346.0698125000004</v>
+        <v>1451.9263002307464</v>
       </c>
       <c r="V13" s="1">
         <v>404.48200000000003</v>
@@ -1550,56 +1660,56 @@
         <v>2506.6260000000002</v>
       </c>
       <c r="AA13" s="1">
-        <f>SUM(C13:F13)</f>
+        <f t="shared" ref="AA13:AA25" si="12">SUM(C13:F13)</f>
         <v>4245.8490000000002</v>
       </c>
       <c r="AB13" s="1">
-        <f>SUM(G13:J13)</f>
+        <f t="shared" ref="AB13:AB25" si="13">SUM(G13:J13)</f>
         <v>4601.8470000000007</v>
       </c>
       <c r="AC13" s="1">
-        <f>SUM(K13:N13)</f>
+        <f t="shared" ref="AC13:AC25" si="14">SUM(K13:N13)</f>
         <v>4606.1149999999998</v>
       </c>
       <c r="AD13" s="1">
         <f>+SUM(O13:R13)</f>
-        <v>4912.9548125000001</v>
+        <v>5292.0243991703192</v>
       </c>
       <c r="AE13" s="1">
         <f>+AE6*AE8</f>
-        <v>5617.9583059782608</v>
+        <v>5679.289728532608</v>
       </c>
       <c r="AF13" s="1">
-        <f t="shared" ref="AF13:AM13" si="11">+AF6*AF8</f>
-        <v>6156.4481960054345</v>
+        <f t="shared" ref="AF13:AM13" si="15">+AF6*AF8</f>
+        <v>6220.8461896874996</v>
       </c>
       <c r="AG13" s="1">
-        <f t="shared" si="11"/>
-        <v>6734.7421792703799</v>
+        <f t="shared" si="15"/>
+        <v>6802.3600726365485</v>
       </c>
       <c r="AH13" s="1">
-        <f t="shared" si="11"/>
-        <v>7355.4744403718068</v>
+        <f t="shared" si="15"/>
+        <v>7426.4732284062839</v>
       </c>
       <c r="AI13" s="1">
-        <f t="shared" si="11"/>
-        <v>8021.4430721352001</v>
+        <f t="shared" si="15"/>
+        <v>8095.9917995714013</v>
       </c>
       <c r="AJ13" s="1">
-        <f t="shared" si="11"/>
-        <v>8735.6198809740035</v>
+        <f t="shared" si="15"/>
+        <v>8813.8960447820136</v>
       </c>
       <c r="AK13" s="1">
-        <f t="shared" si="11"/>
-        <v>9501.1607630163489</v>
+        <f t="shared" si="15"/>
+        <v>9583.3507350147593</v>
       </c>
       <c r="AL13" s="1">
-        <f t="shared" si="11"/>
-        <v>10321.416683560494</v>
+        <f t="shared" si="15"/>
+        <v>10407.716154158825</v>
       </c>
       <c r="AM13" s="1">
-        <f t="shared" si="11"/>
-        <v>11199.945294251513</v>
+        <f t="shared" si="15"/>
+        <v>11290.559738379761</v>
       </c>
     </row>
     <row r="14" spans="1:39">
@@ -1643,20 +1753,19 @@
         <v>621.50400000000002</v>
       </c>
       <c r="O14" s="1">
-        <f>+O$13*(K14/K$13)</f>
-        <v>496.23752791804236</v>
+        <v>574.74900000000002</v>
       </c>
       <c r="P14" s="1">
         <f>+P$13*(L14/L$13)</f>
-        <v>552.62956323542221</v>
+        <v>596.27850896518794</v>
       </c>
       <c r="Q14" s="1">
         <f>+Q$13*(M14/M$13)</f>
-        <v>591.22381010995753</v>
+        <v>637.81830308990413</v>
       </c>
       <c r="R14" s="1">
         <f>+R$13*(N14/N$13)</f>
-        <v>614.55649892197619</v>
+        <v>662.88593316369713</v>
       </c>
       <c r="V14" s="1">
         <v>451.66</v>
@@ -1674,56 +1783,56 @@
         <v>1182.5050000000001</v>
       </c>
       <c r="AA14" s="1">
-        <f>SUM(C14:F14)</f>
+        <f t="shared" si="12"/>
         <v>1751.6020000000001</v>
       </c>
       <c r="AB14" s="1">
-        <f>SUM(G14:J14)</f>
+        <f t="shared" si="13"/>
         <v>1815.3419999999999</v>
       </c>
       <c r="AC14" s="1">
-        <f>SUM(K14:N14)</f>
+        <f t="shared" si="14"/>
         <v>2114.1170000000002</v>
       </c>
       <c r="AD14" s="1">
-        <f t="shared" ref="AD14:AD27" si="12">+SUM(O14:R14)</f>
-        <v>2254.6474001853981</v>
+        <f t="shared" ref="AD14:AD27" si="16">+SUM(O14:R14)</f>
+        <v>2471.7317452187895</v>
       </c>
       <c r="AE14" s="1">
         <f>+AE$13*(AD14/AD$13)</f>
-        <v>2578.1867679093066</v>
+        <v>2652.6107314452042</v>
       </c>
       <c r="AF14" s="1">
-        <f t="shared" ref="AF14:AM14" si="13">+AF$13*(AE14/AE$13)</f>
-        <v>2825.309910073539</v>
+        <f t="shared" ref="AF14:AM14" si="17">+AF$13*(AE14/AE$13)</f>
+        <v>2905.5540657719989</v>
       </c>
       <c r="AG14" s="1">
-        <f t="shared" si="13"/>
-        <v>3090.6998995344215</v>
+        <f t="shared" si="17"/>
+        <v>3177.1602067028593</v>
       </c>
       <c r="AH14" s="1">
-        <f t="shared" si="13"/>
-        <v>3375.5656131662085</v>
+        <f t="shared" si="17"/>
+        <v>3468.6630765623763</v>
       </c>
       <c r="AI14" s="1">
-        <f t="shared" si="13"/>
-        <v>3681.191148412338</v>
+        <f t="shared" si="17"/>
+        <v>3781.3733328910876</v>
       </c>
       <c r="AJ14" s="1">
-        <f t="shared" si="13"/>
-        <v>4008.9403231501651</v>
+        <f t="shared" si="17"/>
+        <v>4116.6829571612634</v>
       </c>
       <c r="AK14" s="1">
-        <f t="shared" si="13"/>
-        <v>4360.2614374907444</v>
+        <f t="shared" si="17"/>
+        <v>4476.0701105262297</v>
       </c>
       <c r="AL14" s="1">
-        <f t="shared" si="13"/>
-        <v>4736.692312457506</v>
+        <f t="shared" si="17"/>
+        <v>4861.1042718347899</v>
       </c>
       <c r="AM14" s="1">
-        <f t="shared" si="13"/>
-        <v>5139.865621327217</v>
+        <f t="shared" si="17"/>
+        <v>5273.4516739978908</v>
       </c>
     </row>
     <row r="15" spans="1:39">
@@ -1767,20 +1876,19 @@
         <v>483.52800000000002</v>
       </c>
       <c r="O15" s="1">
-        <f t="shared" ref="O15:R17" si="14">+O$13*(K15/K$13)</f>
-        <v>513.29736356574097</v>
+        <v>449.75900000000001</v>
       </c>
       <c r="P15" s="1">
-        <f t="shared" si="14"/>
-        <v>531.26284543711586</v>
+        <f t="shared" ref="O15:R17" si="18">+P$13*(L15/L$13)</f>
+        <v>573.22416030590966</v>
       </c>
       <c r="Q15" s="1">
-        <f t="shared" si="14"/>
-        <v>526.12411683638322</v>
+        <f t="shared" si="18"/>
+        <v>567.58808707796425</v>
       </c>
       <c r="R15" s="1">
-        <f t="shared" si="14"/>
-        <v>478.12286777035274</v>
+        <f t="shared" si="18"/>
+        <v>515.72300337693105</v>
       </c>
       <c r="V15" s="1">
         <v>183.67599999999999</v>
@@ -1798,56 +1906,56 @@
         <v>1101.5609999999999</v>
       </c>
       <c r="AA15" s="1">
-        <f>SUM(C15:F15)</f>
+        <f t="shared" si="12"/>
         <v>1699.8329999999999</v>
       </c>
       <c r="AB15" s="1">
-        <f>SUM(G15:J15)</f>
+        <f t="shared" si="13"/>
         <v>2109.8000000000002</v>
       </c>
       <c r="AC15" s="1">
-        <f>SUM(K15:N15)</f>
+        <f t="shared" si="14"/>
         <v>1910.8620000000001</v>
       </c>
       <c r="AD15" s="1">
-        <f t="shared" si="12"/>
-        <v>2048.807193609593</v>
+        <f t="shared" si="16"/>
+        <v>2106.294250760805</v>
       </c>
       <c r="AE15" s="1">
-        <f t="shared" ref="AE15:AM17" si="15">+AE$13*(AD15/AD$13)</f>
-        <v>2342.8087230523502</v>
+        <f t="shared" ref="AE15:AM17" si="19">+AE$13*(AD15/AD$13)</f>
+        <v>2260.4308675312536</v>
       </c>
       <c r="AF15" s="1">
-        <f t="shared" si="15"/>
-        <v>2567.3705198689399</v>
+        <f t="shared" si="19"/>
+        <v>2475.9773530636617</v>
       </c>
       <c r="AG15" s="1">
-        <f t="shared" si="15"/>
-        <v>2808.5314745595579</v>
+        <f t="shared" si="19"/>
+        <v>2707.427409980482</v>
       </c>
       <c r="AH15" s="1">
-        <f t="shared" si="15"/>
-        <v>3067.3900984195657</v>
+        <f t="shared" si="19"/>
+        <v>2955.8325292063255</v>
       </c>
       <c r="AI15" s="1">
-        <f t="shared" si="15"/>
-        <v>3345.1132559791749</v>
+        <f t="shared" si="19"/>
+        <v>3222.3095918298022</v>
       </c>
       <c r="AJ15" s="1">
-        <f t="shared" si="15"/>
-        <v>3642.9402540486963</v>
+        <f t="shared" si="19"/>
+        <v>3508.0447793926105</v>
       </c>
       <c r="AK15" s="1">
-        <f t="shared" si="15"/>
-        <v>3962.1871687852217</v>
+        <f t="shared" si="19"/>
+        <v>3814.2977117321252</v>
       </c>
       <c r="AL15" s="1">
-        <f t="shared" si="15"/>
-        <v>4304.2514243602782</v>
+        <f t="shared" si="19"/>
+        <v>4142.4058253571102</v>
       </c>
       <c r="AM15" s="1">
-        <f t="shared" si="15"/>
-        <v>4670.6166375708772</v>
+        <f t="shared" si="19"/>
+        <v>4493.7890060652635</v>
       </c>
     </row>
     <row r="16" spans="1:39">
@@ -1891,20 +1999,19 @@
         <v>275.81099999999998</v>
       </c>
       <c r="O16" s="1">
-        <f t="shared" si="14"/>
-        <v>302.75174285459963</v>
+        <v>276.03399999999999</v>
       </c>
       <c r="P16" s="1">
-        <f t="shared" si="14"/>
-        <v>312.08354141124261</v>
+        <f t="shared" si="18"/>
+        <v>336.73317738522206</v>
       </c>
       <c r="Q16" s="1">
-        <f t="shared" si="14"/>
-        <v>316.22297815575433</v>
+        <f t="shared" si="18"/>
+        <v>341.14458835449744</v>
       </c>
       <c r="R16" s="1">
-        <f t="shared" si="14"/>
-        <v>272.72783847596986</v>
+        <f t="shared" si="18"/>
+        <v>294.17547129513639</v>
       </c>
       <c r="V16" s="1">
         <v>124.371</v>
@@ -1922,56 +2029,56 @@
         <v>555.46799999999996</v>
       </c>
       <c r="AA16" s="1">
-        <f>SUM(C16:F16)</f>
+        <f t="shared" si="12"/>
         <v>924.41399999999999</v>
       </c>
       <c r="AB16" s="1">
-        <f>SUM(G16:J16)</f>
+        <f t="shared" si="13"/>
         <v>1118.7460000000001</v>
       </c>
       <c r="AC16" s="1">
-        <f>SUM(K16:N16)</f>
+        <f t="shared" si="14"/>
         <v>1122.0919999999999</v>
       </c>
       <c r="AD16" s="1">
-        <f t="shared" si="12"/>
-        <v>1203.7861008975665</v>
+        <f t="shared" si="16"/>
+        <v>1248.0872370348561</v>
       </c>
       <c r="AE16" s="1">
-        <f t="shared" si="15"/>
-        <v>1376.5280533319922</v>
+        <f t="shared" si="19"/>
+        <v>1339.4210780124129</v>
       </c>
       <c r="AF16" s="1">
-        <f t="shared" si="15"/>
-        <v>1508.4703711077007</v>
+        <f t="shared" si="19"/>
+        <v>1467.1434119092771</v>
       </c>
       <c r="AG16" s="1">
-        <f t="shared" si="15"/>
-        <v>1650.1656005276498</v>
+        <f t="shared" si="19"/>
+        <v>1604.2894265007965</v>
       </c>
       <c r="AH16" s="1">
-        <f t="shared" si="15"/>
-        <v>1802.2591769618248</v>
+        <f t="shared" si="19"/>
+        <v>1751.4821840216948</v>
       </c>
       <c r="AI16" s="1">
-        <f t="shared" si="15"/>
-        <v>1965.4366970380981</v>
+        <f t="shared" si="19"/>
+        <v>1909.3834937284307</v>
       </c>
       <c r="AJ16" s="1">
-        <f t="shared" si="15"/>
-        <v>2140.4263211795942</v>
+        <f t="shared" si="19"/>
+        <v>2078.6962289457861</v>
       </c>
       <c r="AK16" s="1">
-        <f t="shared" si="15"/>
-        <v>2328.0013159926448</v>
+        <f t="shared" si="19"/>
+        <v>2260.1667789505559</v>
       </c>
       <c r="AL16" s="1">
-        <f t="shared" si="15"/>
-        <v>2528.9827444840512</v>
+        <f t="shared" si="19"/>
+        <v>2454.5876433834383</v>
       </c>
       <c r="AM16" s="1">
-        <f t="shared" si="15"/>
-        <v>2744.2423125346168</v>
+        <f t="shared" si="19"/>
+        <v>2662.8001773122328</v>
       </c>
     </row>
     <row r="17" spans="2:43">
@@ -2015,20 +2122,19 @@
         <v>229.15700000000001</v>
       </c>
       <c r="O17" s="1">
-        <f t="shared" si="14"/>
-        <v>214.6758017333463</v>
+        <v>227.46299999999999</v>
       </c>
       <c r="P17" s="1">
-        <f t="shared" si="14"/>
-        <v>241.21001279422742</v>
+        <f t="shared" si="18"/>
+        <v>260.26176727563961</v>
       </c>
       <c r="Q17" s="1">
-        <f t="shared" si="14"/>
-        <v>235.15953031043685</v>
+        <f t="shared" si="18"/>
+        <v>253.69251037120154</v>
       </c>
       <c r="R17" s="1">
-        <f t="shared" si="14"/>
-        <v>226.5953616122556</v>
+        <f t="shared" si="18"/>
+        <v>244.41508306622862</v>
       </c>
       <c r="V17" s="1">
         <v>165.16</v>
@@ -2046,56 +2152,56 @@
         <v>529.16399999999999</v>
       </c>
       <c r="AA17" s="1">
-        <f>SUM(C17:F17)</f>
+        <f t="shared" si="12"/>
         <v>780.49699999999996</v>
       </c>
       <c r="AB17" s="1">
-        <f>SUM(G17:J17)</f>
+        <f t="shared" si="13"/>
         <v>953.26499999999999</v>
       </c>
       <c r="AC17" s="1">
-        <f>SUM(K17:N17)</f>
+        <f t="shared" si="14"/>
         <v>857.42300000000012</v>
       </c>
       <c r="AD17" s="1">
-        <f t="shared" si="12"/>
-        <v>917.64070645026618</v>
+        <f t="shared" si="16"/>
+        <v>985.83236071306965</v>
       </c>
       <c r="AE17" s="1">
-        <f t="shared" si="15"/>
-        <v>1049.3211164062648</v>
+        <f t="shared" si="19"/>
+        <v>1057.9746384258112</v>
       </c>
       <c r="AF17" s="1">
-        <f t="shared" si="15"/>
-        <v>1149.9001491797035</v>
+        <f t="shared" si="19"/>
+        <v>1158.8592610748385</v>
       </c>
       <c r="AG17" s="1">
-        <f t="shared" si="15"/>
-        <v>1257.9137824394704</v>
+        <f t="shared" si="19"/>
+        <v>1267.1874093927038</v>
       </c>
       <c r="AH17" s="1">
-        <f t="shared" si="15"/>
-        <v>1373.854028652265</v>
+        <f t="shared" si="19"/>
+        <v>1383.4512243896686</v>
       </c>
       <c r="AI17" s="1">
-        <f t="shared" si="15"/>
-        <v>1498.2435150302401</v>
+        <f t="shared" si="19"/>
+        <v>1508.1734523628481</v>
       </c>
       <c r="AJ17" s="1">
-        <f t="shared" si="15"/>
-        <v>1631.6373149743824</v>
+        <f t="shared" si="19"/>
+        <v>1641.9092750723712</v>
       </c>
       <c r="AK17" s="1">
-        <f t="shared" si="15"/>
-        <v>1774.6248861253632</v>
+        <f t="shared" si="19"/>
+        <v>1785.2482464219397</v>
       </c>
       <c r="AL17" s="1">
-        <f t="shared" si="15"/>
-        <v>1927.8321211040063</v>
+        <f t="shared" si="19"/>
+        <v>1938.8163417187841</v>
       </c>
       <c r="AM17" s="1">
-        <f t="shared" si="15"/>
-        <v>2091.9235173652</v>
+        <f t="shared" si="19"/>
+        <v>2103.2781259292583</v>
       </c>
     </row>
     <row r="18" spans="2:43">
@@ -2103,68 +2209,68 @@
         <v>21</v>
       </c>
       <c r="C18" s="1">
-        <f>+SUM(C14:C17)</f>
+        <f t="shared" ref="C18:R18" si="20">+SUM(C14:C17)</f>
         <v>1073.19</v>
       </c>
       <c r="D18" s="1">
-        <f>+SUM(D14:D17)</f>
+        <f t="shared" si="20"/>
         <v>1511.8489999999999</v>
       </c>
       <c r="E18" s="1">
-        <f>+SUM(E14:E17)</f>
+        <f t="shared" si="20"/>
         <v>1248.2950000000001</v>
       </c>
       <c r="F18" s="1">
-        <f>+SUM(F14:F17)</f>
+        <f t="shared" si="20"/>
         <v>1323.0120000000002</v>
       </c>
       <c r="G18" s="1">
-        <f>+SUM(G14:G17)</f>
+        <f t="shared" si="20"/>
         <v>1334.2539999999999</v>
       </c>
       <c r="H18" s="1">
-        <f>+SUM(H14:H17)</f>
+        <f t="shared" si="20"/>
         <v>1511.8489999999999</v>
       </c>
       <c r="I18" s="1">
-        <f>+SUM(I14:I17)</f>
+        <f t="shared" si="20"/>
         <v>1563.7180000000001</v>
       </c>
       <c r="J18" s="1">
-        <f>+SUM(J14:J17)</f>
+        <f t="shared" si="20"/>
         <v>1587.3319999999999</v>
       </c>
       <c r="K18" s="1">
-        <f>+SUM(K14:K17)</f>
+        <f t="shared" si="20"/>
         <v>1353.8719999999998</v>
       </c>
       <c r="L18" s="1">
-        <f>+SUM(L14:L17)</f>
+        <f t="shared" si="20"/>
         <v>1472.008</v>
       </c>
       <c r="M18" s="1">
-        <f>+SUM(M14:M17)</f>
+        <f t="shared" si="20"/>
         <v>1568.614</v>
       </c>
       <c r="N18" s="1">
-        <f>+SUM(N14:N17)</f>
+        <f t="shared" si="20"/>
         <v>1610</v>
       </c>
       <c r="O18" s="1">
-        <f>+SUM(O14:O17)</f>
-        <v>1526.9624360717294</v>
+        <f t="shared" ref="O18" si="21">+SUM(O14:O17)</f>
+        <v>1528.0049999999999</v>
       </c>
       <c r="P18" s="1">
-        <f>+SUM(P14:P17)</f>
-        <v>1637.185962878008</v>
+        <f t="shared" si="20"/>
+        <v>1766.4976139319592</v>
       </c>
       <c r="Q18" s="1">
-        <f>+SUM(Q14:Q17)</f>
-        <v>1668.730435412532</v>
+        <f t="shared" si="20"/>
+        <v>1800.2434888935672</v>
       </c>
       <c r="R18" s="1">
-        <f>+SUM(R14:R17)</f>
-        <v>1592.0025667805544</v>
+        <f t="shared" si="20"/>
+        <v>1717.1994909019934</v>
       </c>
       <c r="V18" s="1">
         <f>+SUM(V14:V17)</f>
@@ -2187,56 +2293,56 @@
         <v>3368.6979999999994</v>
       </c>
       <c r="AA18" s="1">
-        <f>SUM(C18:F18)</f>
+        <f t="shared" si="12"/>
         <v>5156.3459999999995</v>
       </c>
       <c r="AB18" s="1">
-        <f>SUM(G18:J18)</f>
+        <f t="shared" si="13"/>
         <v>5997.1530000000002</v>
       </c>
       <c r="AC18" s="1">
-        <f>SUM(K18:N18)</f>
+        <f t="shared" si="14"/>
         <v>6004.4940000000006</v>
       </c>
       <c r="AD18" s="1">
-        <f t="shared" si="12"/>
-        <v>6424.881401142824</v>
+        <f t="shared" si="16"/>
+        <v>6811.9455937275188</v>
       </c>
       <c r="AE18" s="1">
         <f>+SUM(AE14:AE17)</f>
-        <v>7346.8446606999141</v>
+        <v>7310.4373154146824</v>
       </c>
       <c r="AF18" s="1">
-        <f t="shared" ref="AF18:AM18" si="16">+SUM(AF14:AF17)</f>
-        <v>8051.0509502298828</v>
+        <f t="shared" ref="AF18:AM18" si="22">+SUM(AF14:AF17)</f>
+        <v>8007.5340918197762</v>
       </c>
       <c r="AG18" s="1">
-        <f t="shared" si="16"/>
-        <v>8807.3107570610991</v>
+        <f t="shared" si="22"/>
+        <v>8756.0644525768421</v>
       </c>
       <c r="AH18" s="1">
-        <f t="shared" si="16"/>
-        <v>9619.0689171998638</v>
+        <f t="shared" si="22"/>
+        <v>9559.4290141800648</v>
       </c>
       <c r="AI18" s="1">
-        <f t="shared" si="16"/>
-        <v>10489.984616459851</v>
+        <f t="shared" si="22"/>
+        <v>10421.239870812167</v>
       </c>
       <c r="AJ18" s="1">
-        <f t="shared" si="16"/>
-        <v>11423.944213352837</v>
+        <f t="shared" si="22"/>
+        <v>11345.333240572032</v>
       </c>
       <c r="AK18" s="1">
-        <f t="shared" si="16"/>
-        <v>12425.074808393972</v>
+        <f t="shared" si="22"/>
+        <v>12335.78284763085</v>
       </c>
       <c r="AL18" s="1">
-        <f t="shared" si="16"/>
-        <v>13497.75860240584</v>
+        <f t="shared" si="22"/>
+        <v>13396.914082294123</v>
       </c>
       <c r="AM18" s="1">
-        <f t="shared" si="16"/>
-        <v>14646.648088797911</v>
+        <f t="shared" si="22"/>
+        <v>14533.318983304645</v>
       </c>
     </row>
     <row r="19" spans="2:43">
@@ -2244,68 +2350,68 @@
         <v>22</v>
       </c>
       <c r="C19" s="1">
-        <f>+C13-C18</f>
+        <f t="shared" ref="C19:R19" si="23">+C13-C18</f>
         <v>-303.60600000000011</v>
       </c>
       <c r="D19" s="1">
-        <f>+D13-D18</f>
+        <f t="shared" si="23"/>
         <v>-400.93999999999983</v>
       </c>
       <c r="E19" s="1">
-        <f>+E13-E18</f>
+        <f t="shared" si="23"/>
         <v>-180.82400000000007</v>
       </c>
       <c r="F19" s="1">
-        <f>+F13-F18</f>
+        <f t="shared" si="23"/>
         <v>-25.12700000000018</v>
       </c>
       <c r="G19" s="1">
-        <f>+G13-G18</f>
+        <f t="shared" si="23"/>
         <v>-271.52699999999982</v>
       </c>
       <c r="H19" s="1">
-        <f>+H13-H18</f>
+        <f t="shared" si="23"/>
         <v>-400.93999999999983</v>
       </c>
       <c r="I19" s="1">
-        <f>+I13-I18</f>
+        <f t="shared" si="23"/>
         <v>-435.24199999999996</v>
       </c>
       <c r="J19" s="1">
-        <f>+J13-J18</f>
+        <f t="shared" si="23"/>
         <v>-287.59699999999998</v>
       </c>
       <c r="K19" s="1">
-        <f>+K13-K18</f>
+        <f t="shared" si="23"/>
         <v>-365.2639999999999</v>
       </c>
       <c r="L19" s="1">
-        <f>+L13-L18</f>
+        <f t="shared" si="23"/>
         <v>-404.33899999999994</v>
       </c>
       <c r="M19" s="1">
-        <f>+M13-M18</f>
+        <f t="shared" si="23"/>
         <v>-380.0630000000001</v>
       </c>
       <c r="N19" s="1">
-        <f>+N13-N18</f>
+        <f t="shared" si="23"/>
         <v>-248.71299999999997</v>
       </c>
       <c r="O19" s="1">
-        <f>+O13-O18</f>
-        <v>-411.96243607172937</v>
+        <f t="shared" ref="O19" si="24">+O13-O18</f>
+        <v>-333.23199999999997</v>
       </c>
       <c r="P19" s="1">
-        <f>+P13-P18</f>
-        <v>-449.71096287800788</v>
+        <f t="shared" si="23"/>
+        <v>-485.23097613575078</v>
       </c>
       <c r="Q19" s="1">
-        <f>+Q13-Q18</f>
-        <v>-404.32043541253188</v>
+        <f t="shared" si="23"/>
+        <v>-436.18502775020238</v>
       </c>
       <c r="R19" s="1">
-        <f>+R13-R18</f>
-        <v>-245.93275428055404</v>
+        <f t="shared" si="23"/>
+        <v>-265.27319067124699</v>
       </c>
       <c r="V19" s="1">
         <f>+V13-V18</f>
@@ -2328,56 +2434,56 @@
         <v>-862.07199999999921</v>
       </c>
       <c r="AA19" s="1">
-        <f>SUM(C19:F19)</f>
+        <f t="shared" si="12"/>
         <v>-910.49700000000018</v>
       </c>
       <c r="AB19" s="1">
-        <f>SUM(G19:J19)</f>
+        <f t="shared" si="13"/>
         <v>-1395.3059999999996</v>
       </c>
       <c r="AC19" s="1">
-        <f>SUM(K19:N19)</f>
+        <f t="shared" si="14"/>
         <v>-1398.3789999999999</v>
       </c>
       <c r="AD19" s="1">
-        <f t="shared" si="12"/>
-        <v>-1511.9265886428232</v>
+        <f t="shared" si="16"/>
+        <v>-1519.9211945572001</v>
       </c>
       <c r="AE19" s="1">
         <f>+AE13-AE18</f>
-        <v>-1728.8863547216533</v>
+        <v>-1631.1475868820744</v>
       </c>
       <c r="AF19" s="1">
-        <f t="shared" ref="AF19:AM19" si="17">+AF13-AF18</f>
-        <v>-1894.6027542244483</v>
+        <f t="shared" ref="AF19:AM19" si="25">+AF13-AF18</f>
+        <v>-1786.6879021322766</v>
       </c>
       <c r="AG19" s="1">
-        <f t="shared" si="17"/>
-        <v>-2072.5685777907192</v>
+        <f t="shared" si="25"/>
+        <v>-1953.7043799402936</v>
       </c>
       <c r="AH19" s="1">
-        <f t="shared" si="17"/>
-        <v>-2263.5944768280569</v>
+        <f t="shared" si="25"/>
+        <v>-2132.9557857737809</v>
       </c>
       <c r="AI19" s="1">
-        <f t="shared" si="17"/>
-        <v>-2468.5415443246511</v>
+        <f t="shared" si="25"/>
+        <v>-2325.248071240766</v>
       </c>
       <c r="AJ19" s="1">
-        <f t="shared" si="17"/>
-        <v>-2688.3243323788338</v>
+        <f t="shared" si="25"/>
+        <v>-2531.4371957900184</v>
       </c>
       <c r="AK19" s="1">
-        <f t="shared" si="17"/>
-        <v>-2923.9140453776236</v>
+        <f t="shared" si="25"/>
+        <v>-2752.4321126160903</v>
       </c>
       <c r="AL19" s="1">
-        <f t="shared" si="17"/>
-        <v>-3176.3419188453463</v>
+        <f t="shared" si="25"/>
+        <v>-2989.1979281352978</v>
       </c>
       <c r="AM19" s="1">
-        <f t="shared" si="17"/>
-        <v>-3446.7027945463979</v>
+        <f t="shared" si="25"/>
+        <v>-3242.7592449248841</v>
       </c>
     </row>
     <row r="20" spans="2:43">
@@ -2421,20 +2527,19 @@
         <v>43.463000000000001</v>
       </c>
       <c r="O20" s="1">
-        <f>+N20</f>
-        <v>43.463000000000001</v>
+        <v>39.898000000000003</v>
       </c>
       <c r="P20" s="1">
-        <f>+O20</f>
-        <v>43.463000000000001</v>
+        <f t="shared" ref="O20:R21" si="26">+O20</f>
+        <v>39.898000000000003</v>
       </c>
       <c r="Q20" s="1">
-        <f>+P20</f>
-        <v>43.463000000000001</v>
+        <f t="shared" si="26"/>
+        <v>39.898000000000003</v>
       </c>
       <c r="R20" s="1">
-        <f>+Q20</f>
-        <v>43.463000000000001</v>
+        <f t="shared" si="26"/>
+        <v>39.898000000000003</v>
       </c>
       <c r="V20" s="1">
         <v>4.6539999999999999</v>
@@ -2452,15 +2557,15 @@
         <v>18.126999999999999</v>
       </c>
       <c r="AA20" s="1">
-        <f>SUM(C20:F20)</f>
+        <f t="shared" si="12"/>
         <v>12.279</v>
       </c>
       <c r="AB20" s="1">
-        <f>SUM(G20:J20)</f>
+        <f t="shared" si="13"/>
         <v>58.597000000000001</v>
       </c>
       <c r="AC20" s="1">
-        <f>SUM(K20:N20)</f>
+        <f t="shared" si="14"/>
         <v>168.39400000000001</v>
       </c>
       <c r="AD20" s="1">
@@ -2468,40 +2573,40 @@
         <v>2.0532000000000017</v>
       </c>
       <c r="AE20" s="1">
-        <f t="shared" ref="AE20:AM20" si="18">+AD46*$AQ$28</f>
-        <v>17.222952940859155</v>
+        <f t="shared" ref="AE20:AM20" si="27">+AD46*$AQ$28</f>
+        <v>17.225156460247796</v>
       </c>
       <c r="AF20" s="1">
-        <f t="shared" si="18"/>
-        <v>35.212048203169822</v>
+        <f t="shared" si="27"/>
+        <v>34.367740225814877</v>
       </c>
       <c r="AG20" s="1">
-        <f t="shared" si="18"/>
-        <v>54.698165986249698</v>
+        <f t="shared" si="27"/>
+        <v>52.926477973453459</v>
       </c>
       <c r="AH20" s="1">
-        <f t="shared" si="18"/>
-        <v>75.79026778062719</v>
+        <f t="shared" si="27"/>
+        <v>73.004308682375012</v>
       </c>
       <c r="AI20" s="1">
-        <f t="shared" si="18"/>
-        <v>98.604425784047876</v>
+        <f t="shared" si="27"/>
+        <v>94.71088207251772</v>
       </c>
       <c r="AJ20" s="1">
-        <f t="shared" si="18"/>
-        <v>123.26426200305858</v>
+        <f t="shared" si="27"/>
+        <v>118.16297276883783</v>
       </c>
       <c r="AK20" s="1">
-        <f t="shared" si="18"/>
-        <v>149.90141348357778</v>
+        <f t="shared" si="27"/>
+        <v>143.48491910069987</v>
       </c>
       <c r="AL20" s="1">
-        <f t="shared" si="18"/>
-        <v>178.65602518564174</v>
+        <f t="shared" si="27"/>
+        <v>170.8090879645107</v>
       </c>
       <c r="AM20" s="1">
-        <f t="shared" si="18"/>
-        <v>209.6772721037116</v>
+        <f t="shared" si="27"/>
+        <v>200.27636725896886</v>
       </c>
     </row>
     <row r="21" spans="2:43">
@@ -2545,21 +2650,20 @@
       <c r="N21" s="1">
         <v>-5.2750000000000004</v>
       </c>
-      <c r="O21" s="1">
-        <f>+N21</f>
-        <v>-5.2750000000000004</v>
+      <c r="O21" s="12">
+        <v>-4.7430000000000003</v>
       </c>
       <c r="P21" s="1">
-        <f>+O21</f>
-        <v>-5.2750000000000004</v>
+        <f t="shared" si="26"/>
+        <v>-4.7430000000000003</v>
       </c>
       <c r="Q21" s="1">
-        <f>+P21</f>
-        <v>-5.2750000000000004</v>
+        <f t="shared" si="26"/>
+        <v>-4.7430000000000003</v>
       </c>
       <c r="R21" s="1">
-        <f>+Q21</f>
-        <v>-5.2750000000000004</v>
+        <f t="shared" si="26"/>
+        <v>-4.7430000000000003</v>
       </c>
       <c r="V21" s="1">
         <v>-1.4239999999999999</v>
@@ -2577,56 +2681,56 @@
         <v>-97.227999999999994</v>
       </c>
       <c r="AA21" s="1">
-        <f>SUM(C21:F21)</f>
+        <f t="shared" si="12"/>
         <v>-18.661000000000001</v>
       </c>
       <c r="AB21" s="1">
-        <f>SUM(G21:J21)</f>
+        <f t="shared" si="13"/>
         <v>-21.459000000000003</v>
       </c>
       <c r="AC21" s="1">
-        <f>SUM(K21:N21)</f>
+        <f t="shared" si="14"/>
         <v>-22.024000000000001</v>
       </c>
       <c r="AD21" s="1">
-        <f t="shared" si="12"/>
-        <v>-21.1</v>
+        <f t="shared" si="16"/>
+        <v>-18.972000000000001</v>
       </c>
       <c r="AE21" s="1">
         <f>+AD21</f>
-        <v>-21.1</v>
+        <v>-18.972000000000001</v>
       </c>
       <c r="AF21" s="1">
-        <f t="shared" ref="AF21:AM21" si="19">+AE21</f>
-        <v>-21.1</v>
+        <f t="shared" ref="AF21:AM21" si="28">+AE21</f>
+        <v>-18.972000000000001</v>
       </c>
       <c r="AG21" s="1">
-        <f t="shared" si="19"/>
-        <v>-21.1</v>
+        <f t="shared" si="28"/>
+        <v>-18.972000000000001</v>
       </c>
       <c r="AH21" s="1">
-        <f t="shared" si="19"/>
-        <v>-21.1</v>
+        <f t="shared" si="28"/>
+        <v>-18.972000000000001</v>
       </c>
       <c r="AI21" s="1">
-        <f t="shared" si="19"/>
-        <v>-21.1</v>
+        <f t="shared" si="28"/>
+        <v>-18.972000000000001</v>
       </c>
       <c r="AJ21" s="1">
-        <f t="shared" si="19"/>
-        <v>-21.1</v>
+        <f t="shared" si="28"/>
+        <v>-18.972000000000001</v>
       </c>
       <c r="AK21" s="1">
-        <f t="shared" si="19"/>
-        <v>-21.1</v>
+        <f t="shared" si="28"/>
+        <v>-18.972000000000001</v>
       </c>
       <c r="AL21" s="1">
-        <f t="shared" si="19"/>
-        <v>-21.1</v>
+        <f t="shared" si="28"/>
+        <v>-18.972000000000001</v>
       </c>
       <c r="AM21" s="1">
-        <f t="shared" si="19"/>
-        <v>-21.1</v>
+        <f t="shared" si="28"/>
+        <v>-18.972000000000001</v>
       </c>
     </row>
     <row r="22" spans="2:43">
@@ -2670,7 +2774,8 @@
         <v>-34.447000000000003</v>
       </c>
       <c r="O22" s="1">
-        <v>-34.447000000000003</v>
+        <f>+-0.081</f>
+        <v>-8.1000000000000003E-2</v>
       </c>
       <c r="P22" s="1">
         <v>-34.447000000000003</v>
@@ -2697,15 +2802,15 @@
         <v>14.988</v>
       </c>
       <c r="AA22" s="1">
-        <f>SUM(C22:F22)</f>
+        <f t="shared" si="12"/>
         <v>180.983</v>
       </c>
       <c r="AB22" s="1">
-        <f>SUM(G22:J22)</f>
+        <f t="shared" si="13"/>
         <v>-42.529000000000003</v>
       </c>
       <c r="AC22" s="1">
-        <f>SUM(K22:N22)</f>
+        <f t="shared" si="14"/>
         <v>-42.414000000000001</v>
       </c>
       <c r="AD22" s="1">
@@ -2713,39 +2818,39 @@
         <v>-42.414000000000001</v>
       </c>
       <c r="AE22" s="1">
-        <f t="shared" ref="AE22:AM22" si="20">+AD22</f>
+        <f t="shared" ref="AE22:AM22" si="29">+AD22</f>
         <v>-42.414000000000001</v>
       </c>
       <c r="AF22" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>-42.414000000000001</v>
       </c>
       <c r="AG22" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>-42.414000000000001</v>
       </c>
       <c r="AH22" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>-42.414000000000001</v>
       </c>
       <c r="AI22" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>-42.414000000000001</v>
       </c>
       <c r="AJ22" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>-42.414000000000001</v>
       </c>
       <c r="AK22" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>-42.414000000000001</v>
       </c>
       <c r="AL22" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>-42.414000000000001</v>
       </c>
       <c r="AM22" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>-42.414000000000001</v>
       </c>
     </row>
@@ -2754,68 +2859,68 @@
         <v>26</v>
       </c>
       <c r="C23" s="1">
-        <f>+SUM(C19:C22)</f>
+        <f t="shared" ref="C23:R23" si="30">+SUM(C19:C22)</f>
         <v>-285.44200000000012</v>
       </c>
       <c r="D23" s="1">
-        <f>+SUM(D19:D22)</f>
+        <f t="shared" si="30"/>
         <v>-415.06799999999981</v>
       </c>
       <c r="E23" s="1">
-        <f>+SUM(E19:E22)</f>
+        <f t="shared" si="30"/>
         <v>-70.96700000000007</v>
       </c>
       <c r="F23" s="1">
-        <f>+SUM(F19:F22)</f>
+        <f t="shared" si="30"/>
         <v>35.580999999999818</v>
       </c>
       <c r="G23" s="1">
-        <f>+SUM(G19:G22)</f>
+        <f t="shared" si="30"/>
         <v>-351.11399999999981</v>
       </c>
       <c r="H23" s="1">
-        <f>+SUM(H19:H22)</f>
+        <f t="shared" si="30"/>
         <v>-415.06799999999981</v>
       </c>
       <c r="I23" s="1">
-        <f>+SUM(I19:I22)</f>
+        <f t="shared" si="30"/>
         <v>-350.26099999999997</v>
       </c>
       <c r="J23" s="1">
-        <f>+SUM(J19:J22)</f>
+        <f t="shared" si="30"/>
         <v>-284.25400000000002</v>
       </c>
       <c r="K23" s="1">
-        <f>+SUM(K19:K22)</f>
+        <f t="shared" si="30"/>
         <v>-321.82899999999989</v>
       </c>
       <c r="L23" s="1">
-        <f>+SUM(L19:L22)</f>
+        <f t="shared" si="30"/>
         <v>-365.21499999999997</v>
       </c>
       <c r="M23" s="1">
-        <f>+SUM(M19:M22)</f>
+        <f t="shared" si="30"/>
         <v>-362.4070000000001</v>
       </c>
       <c r="N23" s="1">
-        <f>+SUM(N19:N22)</f>
+        <f t="shared" si="30"/>
         <v>-244.97199999999998</v>
       </c>
       <c r="O23" s="1">
-        <f>+SUM(O19:O22)</f>
-        <v>-408.22143607172933</v>
+        <f t="shared" ref="O23" si="31">+SUM(O19:O22)</f>
+        <v>-298.15799999999996</v>
       </c>
       <c r="P23" s="1">
-        <f>+SUM(P19:P22)</f>
-        <v>-445.96996287800783</v>
+        <f t="shared" si="30"/>
+        <v>-484.52297613575075</v>
       </c>
       <c r="Q23" s="1">
-        <f>+SUM(Q19:Q22)</f>
-        <v>-400.57943541253184</v>
+        <f t="shared" si="30"/>
+        <v>-435.47702775020235</v>
       </c>
       <c r="R23" s="1">
-        <f>+SUM(R19:R22)</f>
-        <v>-242.19175428055405</v>
+        <f t="shared" si="30"/>
+        <v>-264.56519067124702</v>
       </c>
       <c r="V23" s="1">
         <f>+SUM(V19:V22)</f>
@@ -2838,56 +2943,56 @@
         <v>-926.18499999999926</v>
       </c>
       <c r="AA23" s="1">
-        <f>SUM(C23:F23)</f>
+        <f t="shared" si="12"/>
         <v>-735.8960000000003</v>
       </c>
       <c r="AB23" s="1">
-        <f>SUM(G23:J23)</f>
+        <f t="shared" si="13"/>
         <v>-1400.6969999999997</v>
       </c>
       <c r="AC23" s="1">
-        <f>SUM(K23:N23)</f>
+        <f t="shared" si="14"/>
         <v>-1294.423</v>
       </c>
       <c r="AD23" s="1">
-        <f t="shared" si="12"/>
-        <v>-1496.962588642823</v>
+        <f t="shared" si="16"/>
+        <v>-1482.7231945572003</v>
       </c>
       <c r="AE23" s="1">
         <f>+SUM(AE19:AE22)</f>
-        <v>-1775.1774017807941</v>
+        <v>-1675.3084304218266</v>
       </c>
       <c r="AF23" s="1">
-        <f t="shared" ref="AF23:AM23" si="21">+SUM(AF19:AF22)</f>
-        <v>-1922.9047060212783</v>
+        <f t="shared" ref="AF23:AM23" si="32">+SUM(AF19:AF22)</f>
+        <v>-1813.7061619064616</v>
       </c>
       <c r="AG23" s="1">
-        <f t="shared" si="21"/>
-        <v>-2081.3844118044694</v>
+        <f t="shared" si="32"/>
+        <v>-1962.1639019668401</v>
       </c>
       <c r="AH23" s="1">
-        <f t="shared" si="21"/>
-        <v>-2251.3182090474297</v>
+        <f t="shared" si="32"/>
+        <v>-2121.3374770914065</v>
       </c>
       <c r="AI23" s="1">
-        <f t="shared" si="21"/>
-        <v>-2433.4511185406031</v>
+        <f t="shared" si="32"/>
+        <v>-2291.9231891682489</v>
       </c>
       <c r="AJ23" s="1">
-        <f t="shared" si="21"/>
-        <v>-2628.5740703757751</v>
+        <f t="shared" si="32"/>
+        <v>-2474.6602230211811</v>
       </c>
       <c r="AK23" s="1">
-        <f t="shared" si="21"/>
-        <v>-2837.5266318940457</v>
+        <f t="shared" si="32"/>
+        <v>-2670.333193515391</v>
       </c>
       <c r="AL23" s="1">
-        <f t="shared" si="21"/>
-        <v>-3061.1998936597047</v>
+        <f t="shared" si="32"/>
+        <v>-2879.7748401707877</v>
       </c>
       <c r="AM23" s="1">
-        <f t="shared" si="21"/>
-        <v>-3300.5395224426866</v>
+        <f t="shared" si="32"/>
+        <v>-3103.8688776659155</v>
       </c>
     </row>
     <row r="24" spans="2:43">
@@ -2931,20 +3036,19 @@
         <v>-3.2749999999999999</v>
       </c>
       <c r="O24" s="1">
-        <f>+O23*(N24/N23)</f>
-        <v>-5.4574612736758228</v>
+        <v>-6.9320000000000004</v>
       </c>
       <c r="P24" s="1">
         <f>+P23*(O24/O23)</f>
-        <v>-5.9621166028177743</v>
+        <v>-11.264877248214118</v>
       </c>
       <c r="Q24" s="1">
         <f>+Q23*(P24/P23)</f>
-        <v>-5.3552963235636799</v>
+        <v>-10.124587488393415</v>
       </c>
       <c r="R24" s="1">
         <f>+R23*(Q24/Q23)</f>
-        <v>-3.2378312430351821</v>
+        <v>-6.1509867309717832</v>
       </c>
       <c r="V24" s="1">
         <v>7.08</v>
@@ -2962,56 +3066,56 @@
         <v>-18.654</v>
       </c>
       <c r="AA24" s="1">
-        <f>SUM(C24:F24)</f>
+        <f t="shared" si="12"/>
         <v>-22.462000000000003</v>
       </c>
       <c r="AB24" s="1">
-        <f>SUM(G24:J24)</f>
+        <f t="shared" si="13"/>
         <v>-31.594999999999999</v>
       </c>
       <c r="AC24" s="1">
-        <f>SUM(K24:N24)</f>
+        <f t="shared" si="14"/>
         <v>-28.061999999999998</v>
       </c>
       <c r="AD24" s="1">
-        <f t="shared" si="12"/>
-        <v>-20.012705443092457</v>
+        <f t="shared" si="16"/>
+        <v>-34.472451467579312</v>
       </c>
       <c r="AE24" s="1">
         <f>+AE23*(AD24/AD23)</f>
-        <v>-23.732124450272281</v>
+        <v>-38.949946134881849</v>
       </c>
       <c r="AF24" s="1">
-        <f t="shared" ref="AF24:AM24" si="22">+AF23*(AE24/AE23)</f>
-        <v>-25.707072286709039</v>
+        <f t="shared" ref="AF24:AM24" si="33">+AF23*(AE24/AE23)</f>
+        <v>-42.167612857396385</v>
       </c>
       <c r="AG24" s="1">
-        <f t="shared" si="22"/>
-        <v>-27.825767633279057</v>
+        <f t="shared" si="33"/>
+        <v>-45.619168925315215</v>
       </c>
       <c r="AH24" s="1">
-        <f t="shared" si="22"/>
-        <v>-30.097591294639109</v>
+        <f t="shared" si="33"/>
+        <v>-49.319861922865158</v>
       </c>
       <c r="AI24" s="1">
-        <f t="shared" si="22"/>
-        <v>-32.532503360467622</v>
+        <f t="shared" si="33"/>
+        <v>-53.285880463761835</v>
       </c>
       <c r="AJ24" s="1">
-        <f t="shared" si="22"/>
-        <v>-35.141077676145279</v>
+        <f t="shared" si="33"/>
+        <v>-57.534410165022663</v>
       </c>
       <c r="AK24" s="1">
-        <f t="shared" si="22"/>
-        <v>-37.934538312349972</v>
+        <f t="shared" si="33"/>
+        <v>-62.083692865690978</v>
       </c>
       <c r="AL24" s="1">
-        <f t="shared" si="22"/>
-        <v>-40.924798147280221</v>
+        <f t="shared" si="33"/>
+        <v>-66.953089275028333</v>
       </c>
       <c r="AM24" s="1">
-        <f t="shared" si="22"/>
-        <v>-44.124499681595431</v>
+        <f t="shared" si="33"/>
+        <v>-72.163145245071817</v>
       </c>
     </row>
     <row r="25" spans="2:43">
@@ -3019,67 +3123,67 @@
         <v>28</v>
       </c>
       <c r="C25" s="1">
-        <f>+SUM(C23:C24)</f>
+        <f t="shared" ref="C25:I25" si="34">+SUM(C23:C24)</f>
         <v>-286.88200000000012</v>
       </c>
       <c r="D25" s="1">
-        <f>+SUM(D23:D24)</f>
+        <f t="shared" si="34"/>
         <v>-422.06699999999984</v>
       </c>
       <c r="E25" s="1">
-        <f>+SUM(E23:E24)</f>
+        <f t="shared" si="34"/>
         <v>-71.959000000000074</v>
       </c>
       <c r="F25" s="1">
-        <f>+SUM(F23:F24)</f>
+        <f t="shared" si="34"/>
         <v>22.54999999999982</v>
       </c>
       <c r="G25" s="1">
-        <f>+SUM(G23:G24)</f>
+        <f t="shared" si="34"/>
         <v>-359.6239999999998</v>
       </c>
       <c r="H25" s="1">
-        <f>+SUM(H23:H24)</f>
+        <f t="shared" si="34"/>
         <v>-422.06699999999984</v>
       </c>
       <c r="I25" s="1">
-        <f>+SUM(I23:I24)</f>
+        <f t="shared" si="34"/>
         <v>-359.50199999999995</v>
       </c>
       <c r="J25" s="1">
         <v>-4.2060000000000004</v>
       </c>
       <c r="K25" s="1">
-        <f>+SUM(K23:K24)</f>
+        <f t="shared" ref="K25:R25" si="35">+SUM(K23:K24)</f>
         <v>-328.67399999999992</v>
       </c>
       <c r="L25" s="1">
-        <f>+SUM(L23:L24)</f>
+        <f t="shared" si="35"/>
         <v>-377.30799999999999</v>
       </c>
       <c r="M25" s="1">
-        <f>+SUM(M23:M24)</f>
+        <f t="shared" si="35"/>
         <v>-368.25600000000009</v>
       </c>
       <c r="N25" s="1">
-        <f>+SUM(N23:N24)</f>
+        <f t="shared" si="35"/>
         <v>-248.24699999999999</v>
       </c>
       <c r="O25" s="1">
-        <f>+SUM(O23:O24)</f>
-        <v>-413.67889734540518</v>
+        <f t="shared" ref="O25" si="36">+SUM(O23:O24)</f>
+        <v>-305.08999999999997</v>
       </c>
       <c r="P25" s="1">
-        <f>+SUM(P23:P24)</f>
-        <v>-451.93207948082562</v>
+        <f t="shared" si="35"/>
+        <v>-495.78785338396489</v>
       </c>
       <c r="Q25" s="1">
-        <f>+SUM(Q23:Q24)</f>
-        <v>-405.9347317360955</v>
+        <f t="shared" si="35"/>
+        <v>-445.60161523859574</v>
       </c>
       <c r="R25" s="1">
-        <f>+SUM(R23:R24)</f>
-        <v>-245.42958552358922</v>
+        <f t="shared" si="35"/>
+        <v>-270.71617740221882</v>
       </c>
       <c r="V25" s="1">
         <f>+SUM(V23:V24)</f>
@@ -3102,56 +3206,56 @@
         <v>-944.83899999999926</v>
       </c>
       <c r="AA25" s="1">
-        <f>SUM(C25:F25)</f>
+        <f t="shared" si="12"/>
         <v>-758.35800000000017</v>
       </c>
       <c r="AB25" s="1">
-        <f>SUM(G25:J25)</f>
+        <f t="shared" si="13"/>
         <v>-1145.3989999999994</v>
       </c>
       <c r="AC25" s="1">
-        <f>SUM(K25:N25)</f>
+        <f t="shared" si="14"/>
         <v>-1322.4850000000001</v>
       </c>
       <c r="AD25" s="1">
-        <f t="shared" si="12"/>
-        <v>-1516.9752940859155</v>
+        <f t="shared" si="16"/>
+        <v>-1517.1956460247793</v>
       </c>
       <c r="AE25" s="1">
         <f>+SUM(AE23:AE24)</f>
-        <v>-1798.9095262310664</v>
+        <v>-1714.2583765567085</v>
       </c>
       <c r="AF25" s="1">
-        <f t="shared" ref="AF25:AM25" si="23">+SUM(AF23:AF24)</f>
-        <v>-1948.6117783079874</v>
+        <f t="shared" ref="AF25:AM25" si="37">+SUM(AF23:AF24)</f>
+        <v>-1855.8737747638579</v>
       </c>
       <c r="AG25" s="1">
-        <f t="shared" si="23"/>
-        <v>-2109.2101794377486</v>
+        <f t="shared" si="37"/>
+        <v>-2007.7830708921554</v>
       </c>
       <c r="AH25" s="1">
-        <f t="shared" si="23"/>
-        <v>-2281.4158003420689</v>
+        <f t="shared" si="37"/>
+        <v>-2170.6573390142717</v>
       </c>
       <c r="AI25" s="1">
-        <f t="shared" si="23"/>
-        <v>-2465.9836219010708</v>
+        <f t="shared" si="37"/>
+        <v>-2345.2090696320106</v>
       </c>
       <c r="AJ25" s="1">
-        <f t="shared" si="23"/>
-        <v>-2663.7151480519206</v>
+        <f t="shared" si="37"/>
+        <v>-2532.1946331862036</v>
       </c>
       <c r="AK25" s="1">
-        <f t="shared" si="23"/>
-        <v>-2875.4611702063958</v>
+        <f t="shared" si="37"/>
+        <v>-2732.4168863810819</v>
       </c>
       <c r="AL25" s="1">
-        <f t="shared" si="23"/>
-        <v>-3102.1246918069851</v>
+        <f t="shared" si="37"/>
+        <v>-2946.7279294458158</v>
       </c>
       <c r="AM25" s="1">
-        <f t="shared" si="23"/>
-        <v>-3344.6640221242819</v>
+        <f t="shared" si="37"/>
+        <v>-3176.0320229109875</v>
       </c>
     </row>
     <row r="26" spans="2:43">
@@ -3195,20 +3299,19 @@
         <v>1638.7139999999999</v>
       </c>
       <c r="O26" s="1">
-        <f>+N26</f>
-        <v>1638.7139999999999</v>
+        <v>1647.3869999999999</v>
       </c>
       <c r="P26" s="1">
         <f>+O26</f>
-        <v>1638.7139999999999</v>
+        <v>1647.3869999999999</v>
       </c>
       <c r="Q26" s="1">
         <f>+P26</f>
-        <v>1638.7139999999999</v>
+        <v>1647.3869999999999</v>
       </c>
       <c r="R26" s="1">
         <f>+Q26</f>
-        <v>1638.7139999999999</v>
+        <v>1647.3869999999999</v>
       </c>
       <c r="V26" s="1">
         <f>+V25/V27</f>
@@ -3241,43 +3344,43 @@
       </c>
       <c r="AD26" s="1">
         <f>+AD25/AD27</f>
-        <v>1638.7139999999999</v>
+        <v>1647.3869999999999</v>
       </c>
       <c r="AE26" s="1">
         <f>+AD26</f>
-        <v>1638.7139999999999</v>
+        <v>1647.3869999999999</v>
       </c>
       <c r="AF26" s="1">
-        <f t="shared" ref="AF26:AM26" si="24">+AE26</f>
-        <v>1638.7139999999999</v>
+        <f t="shared" ref="AF26:AM26" si="38">+AE26</f>
+        <v>1647.3869999999999</v>
       </c>
       <c r="AG26" s="1">
-        <f t="shared" si="24"/>
-        <v>1638.7139999999999</v>
+        <f t="shared" si="38"/>
+        <v>1647.3869999999999</v>
       </c>
       <c r="AH26" s="1">
-        <f t="shared" si="24"/>
-        <v>1638.7139999999999</v>
+        <f t="shared" si="38"/>
+        <v>1647.3869999999999</v>
       </c>
       <c r="AI26" s="1">
-        <f t="shared" si="24"/>
-        <v>1638.7139999999999</v>
+        <f t="shared" si="38"/>
+        <v>1647.3869999999999</v>
       </c>
       <c r="AJ26" s="1">
-        <f t="shared" si="24"/>
-        <v>1638.7139999999999</v>
+        <f t="shared" si="38"/>
+        <v>1647.3869999999999</v>
       </c>
       <c r="AK26" s="1">
-        <f t="shared" si="24"/>
-        <v>1638.7139999999999</v>
+        <f t="shared" si="38"/>
+        <v>1647.3869999999999</v>
       </c>
       <c r="AL26" s="1">
-        <f t="shared" si="24"/>
-        <v>1638.7139999999999</v>
+        <f t="shared" si="38"/>
+        <v>1647.3869999999999</v>
       </c>
       <c r="AM26" s="1">
-        <f t="shared" si="24"/>
-        <v>1638.7139999999999</v>
+        <f t="shared" si="38"/>
+        <v>1647.3869999999999</v>
       </c>
     </row>
     <row r="27" spans="2:43" s="6" customFormat="1">
@@ -3285,68 +3388,68 @@
         <v>30</v>
       </c>
       <c r="C27" s="6">
-        <f>+C25/C26</f>
+        <f t="shared" ref="C27:R27" si="39">+C25/C26</f>
         <v>-0.19104629883673549</v>
       </c>
       <c r="D27" s="6">
-        <f>+D25/D26</f>
+        <f t="shared" si="39"/>
         <v>-0.25859730170205975</v>
       </c>
       <c r="E27" s="6">
-        <f>+E25/E26</f>
+        <f t="shared" si="39"/>
         <v>-4.5515842845450238E-2</v>
       </c>
       <c r="F27" s="6">
-        <f>+F25/F26</f>
+        <f t="shared" si="39"/>
         <v>1.3512064086131962E-2</v>
       </c>
       <c r="G27" s="6">
-        <f>+G25/G26</f>
+        <f t="shared" si="39"/>
         <v>-0.22211173648781757</v>
       </c>
       <c r="H27" s="6">
-        <f>+H25/H26</f>
+        <f t="shared" si="39"/>
         <v>-0.25859730170205975</v>
       </c>
       <c r="I27" s="6">
-        <f>+I25/I26</f>
+        <f t="shared" si="39"/>
         <v>-0.22349820300984194</v>
       </c>
       <c r="J27" s="6">
-        <f>+J25/J26</f>
+        <f t="shared" si="39"/>
         <v>-2.6723714532782936E-3</v>
       </c>
       <c r="K27" s="6">
-        <f>+K25/K26</f>
+        <f t="shared" si="39"/>
         <v>-0.20784130216204932</v>
       </c>
       <c r="L27" s="6">
-        <f>+L25/L26</f>
+        <f t="shared" si="39"/>
         <v>-0.23535091680742926</v>
       </c>
       <c r="M27" s="6">
-        <f>+M25/M26</f>
+        <f t="shared" si="39"/>
         <v>-0.22649126615934276</v>
       </c>
       <c r="N27" s="6">
-        <f>+N25/N26</f>
+        <f t="shared" si="39"/>
         <v>-0.15148891142688717</v>
       </c>
       <c r="O27" s="6">
-        <f>+O25/O26</f>
-        <v>-0.25244118091711254</v>
+        <f t="shared" ref="O27" si="40">+O25/O26</f>
+        <v>-0.18519631392016569</v>
       </c>
       <c r="P27" s="6">
-        <f>+P25/P26</f>
-        <v>-0.27578459662932375</v>
+        <f t="shared" si="39"/>
+        <v>-0.30095408873808333</v>
       </c>
       <c r="Q27" s="6">
-        <f>+Q25/Q26</f>
-        <v>-0.2477154230305566</v>
+        <f t="shared" si="39"/>
+        <v>-0.27048994270234972</v>
       </c>
       <c r="R27" s="6">
-        <f>+R25/R26</f>
-        <v>-0.14976962760041668</v>
+        <f t="shared" si="39"/>
+        <v>-0.16433065054065549</v>
       </c>
       <c r="V27" s="6">
         <v>-0.64</v>
@@ -3379,44 +3482,44 @@
         <v>-0.82117239655570851</v>
       </c>
       <c r="AD27" s="1">
-        <f t="shared" si="12"/>
-        <v>-0.92571082817740957</v>
+        <f t="shared" si="16"/>
+        <v>-0.9209709959012542</v>
       </c>
       <c r="AE27" s="6">
         <f>+AE25/AE26</f>
-        <v>-1.0977568546012706</v>
+        <v>-1.0405923905898908</v>
       </c>
       <c r="AF27" s="6">
-        <f t="shared" ref="AF27:AM27" si="25">+AF25/AF26</f>
-        <v>-1.1891103501330844</v>
+        <f t="shared" ref="AF27:AM27" si="41">+AF25/AF26</f>
+        <v>-1.1265560398156949</v>
       </c>
       <c r="AG27" s="6">
-        <f t="shared" si="25"/>
-        <v>-1.2871130529413606</v>
+        <f t="shared" si="41"/>
+        <v>-1.2187683105986362</v>
       </c>
       <c r="AH27" s="6">
-        <f t="shared" si="25"/>
-        <v>-1.3921988829912169</v>
+        <f t="shared" si="41"/>
+        <v>-1.3176365596027355</v>
       </c>
       <c r="AI27" s="6">
-        <f t="shared" si="25"/>
-        <v>-1.5048285557461953</v>
+        <f t="shared" si="41"/>
+        <v>-1.4235932841718495</v>
       </c>
       <c r="AJ27" s="6">
-        <f t="shared" si="25"/>
-        <v>-1.6254911766494462</v>
+        <f t="shared" si="41"/>
+        <v>-1.5370976177341473</v>
       </c>
       <c r="AK27" s="6">
-        <f t="shared" si="25"/>
-        <v>-1.7547059280670061</v>
+        <f t="shared" si="41"/>
+        <v>-1.6586369118981041</v>
       </c>
       <c r="AL27" s="6">
-        <f t="shared" si="25"/>
-        <v>-1.8930238539531519</v>
+        <f t="shared" si="41"/>
+        <v>-1.7887284101706618</v>
       </c>
       <c r="AM27" s="6">
-        <f t="shared" si="25"/>
-        <v>-2.0410297477926482</v>
+        <f t="shared" si="41"/>
+        <v>-1.9279210185044484</v>
       </c>
     </row>
     <row r="28" spans="2:43">
@@ -3433,7 +3536,7 @@
       </c>
       <c r="AQ29" s="1">
         <f>+AE13</f>
-        <v>5617.9583059782608</v>
+        <v>5679.289728532608</v>
       </c>
     </row>
     <row r="30" spans="2:43">
@@ -3442,7 +3545,7 @@
       </c>
       <c r="AQ30" s="10">
         <f>+Main!G9/Model!AQ29</f>
-        <v>3.3096285376511565</v>
+        <v>4.6948626508598998</v>
       </c>
     </row>
     <row r="31" spans="2:43">
@@ -3454,7 +3557,7 @@
       </c>
       <c r="AQ31" s="1">
         <f>+AQ29*AQ30</f>
-        <v>18593.355132799999</v>
+        <v>26663.485229900001</v>
       </c>
     </row>
     <row r="32" spans="2:43" s="7" customFormat="1">
@@ -3462,127 +3565,127 @@
         <v>18</v>
       </c>
       <c r="G32" s="7">
-        <f>+G13/C13-1</f>
+        <f t="shared" ref="G32:R36" si="42">+G13/C13-1</f>
         <v>0.38091098567537807</v>
       </c>
       <c r="H32" s="7">
-        <f>+H13/D13-1</f>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="I32" s="7">
-        <f>+I13/E13-1</f>
+        <f t="shared" si="42"/>
         <v>5.7149093511673854E-2</v>
       </c>
       <c r="J32" s="7">
-        <f>+J13/F13-1</f>
+        <f t="shared" si="42"/>
         <v>1.4253959326133714E-3</v>
       </c>
       <c r="K32" s="7">
-        <f>+K13/G13-1</f>
+        <f t="shared" si="42"/>
         <v>-6.9744158189262273E-2</v>
       </c>
       <c r="L32" s="7">
-        <f>+L13/H13-1</f>
+        <f t="shared" si="42"/>
         <v>-3.8923080108271724E-2</v>
       </c>
       <c r="M32" s="7">
-        <f>+M13/I13-1</f>
+        <f t="shared" si="42"/>
         <v>5.3235514091571012E-2</v>
       </c>
       <c r="N32" s="7">
-        <f>+N13/J13-1</f>
+        <f t="shared" si="42"/>
         <v>4.7357345920514771E-2</v>
       </c>
       <c r="O32" s="7">
-        <f>+O13/K13-1</f>
-        <v>0.12784844953712704</v>
+        <f t="shared" si="42"/>
+        <v>0.20854069560432453</v>
       </c>
       <c r="P32" s="7">
-        <f>+P13/L13-1</f>
-        <v>0.11221268014712438</v>
+        <f t="shared" si="42"/>
+        <v>0.20005979174838684</v>
       </c>
       <c r="Q32" s="7">
-        <f>+Q13/M13-1</f>
-        <v>6.3824774872933698E-2</v>
+        <f t="shared" si="42"/>
+        <v>0.14766506539758484</v>
       </c>
       <c r="R32" s="7">
-        <f>+R13/N13-1</f>
-        <v>-1.1178529949966265E-2</v>
+        <f t="shared" si="42"/>
+        <v>6.6583534721734949E-2</v>
       </c>
       <c r="W32" s="7">
-        <f>+W13/V13-1</f>
+        <f t="shared" ref="W32:AM32" si="43">+W13/V13-1</f>
         <v>1.0395196819635975</v>
       </c>
       <c r="X32" s="7">
-        <f>+X13/W13-1</f>
+        <f t="shared" si="43"/>
         <v>0.43093209398399179</v>
       </c>
       <c r="Y32" s="7">
-        <f>+Y13/X13-1</f>
+        <f t="shared" si="43"/>
         <v>0.45329307736228519</v>
       </c>
       <c r="Z32" s="7">
-        <f>+Z13/Y13-1</f>
+        <f t="shared" si="43"/>
         <v>0.4611345505247928</v>
       </c>
       <c r="AA32" s="7">
-        <f>+AA13/Z13-1</f>
+        <f t="shared" si="43"/>
         <v>0.69385021937855895</v>
       </c>
       <c r="AB32" s="7">
-        <f>+AB13/AA13-1</f>
+        <f t="shared" si="43"/>
         <v>8.3846128300841816E-2</v>
       </c>
       <c r="AC32" s="7">
-        <f>+AC13/AB13-1</f>
+        <f t="shared" si="43"/>
         <v>9.2745369413615997E-4</v>
       </c>
       <c r="AD32" s="7">
-        <f>+AD13/AC13-1</f>
-        <v>6.6615751560697101E-2</v>
+        <f t="shared" si="43"/>
+        <v>0.14891278206695224</v>
       </c>
       <c r="AE32" s="7">
-        <f>+AE13/AD13-1</f>
-        <v>0.14349887600930589</v>
+        <f t="shared" si="43"/>
+        <v>7.3179052126631117E-2</v>
       </c>
       <c r="AF32" s="7">
-        <f>+AF13/AE13-1</f>
-        <v>9.585152838427935E-2</v>
+        <f t="shared" si="43"/>
+        <v>9.5356371490280756E-2</v>
       </c>
       <c r="AG32" s="7">
-        <f>+AG13/AF13-1</f>
-        <v>9.393305439330546E-2</v>
+        <f t="shared" si="43"/>
+        <v>9.3478260869565233E-2</v>
       </c>
       <c r="AH32" s="7">
-        <f>+AH13/AG13-1</f>
-        <v>9.2168674698795305E-2</v>
+        <f t="shared" si="43"/>
+        <v>9.1749502982107378E-2</v>
       </c>
       <c r="AI32" s="7">
-        <f>+AI13/AH13-1</f>
-        <v>9.0540540540540615E-2</v>
+        <f t="shared" si="43"/>
+        <v>9.0152963671128239E-2</v>
       </c>
       <c r="AJ32" s="7">
-        <f>+AJ13/AI13-1</f>
-        <v>8.9033457249070747E-2</v>
+        <f t="shared" si="43"/>
+        <v>8.8674033149171105E-2</v>
       </c>
       <c r="AK32" s="7">
-        <f>+AK13/AJ13-1</f>
-        <v>8.7634408602150549E-2</v>
+        <f t="shared" si="43"/>
+        <v>8.7300177619893393E-2</v>
       </c>
       <c r="AL32" s="7">
-        <f>+AL13/AK13-1</f>
-        <v>8.6332179930795894E-2</v>
+        <f t="shared" si="43"/>
+        <v>8.6020583190394406E-2</v>
       </c>
       <c r="AM32" s="7">
-        <f>+AM13/AL13-1</f>
-        <v>8.5117056856187423E-2</v>
+        <f t="shared" si="43"/>
+        <v>8.4825870646766388E-2</v>
       </c>
       <c r="AP32" s="7" t="s">
         <v>68</v>
       </c>
       <c r="AQ32" s="1">
         <f>+Main!G5</f>
-        <v>1650.6315199999999</v>
+        <v>1641.0389899999998</v>
       </c>
     </row>
     <row r="33" spans="2:43" s="7" customFormat="1">
@@ -3590,127 +3693,127 @@
         <v>3</v>
       </c>
       <c r="G33" s="7">
-        <f>+G14/C14-1</f>
+        <f t="shared" si="42"/>
         <v>2.0106592082908215E-2</v>
       </c>
       <c r="H33" s="7">
-        <f>+H14/D14-1</f>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="I33" s="7">
-        <f>+I14/E14-1</f>
+        <f t="shared" si="42"/>
         <v>5.2503760093624674E-2</v>
       </c>
       <c r="J33" s="7">
-        <f>+J14/F14-1</f>
+        <f t="shared" si="42"/>
         <v>7.1601755311687887E-2</v>
       </c>
       <c r="K33" s="7">
-        <f>+K14/G14-1</f>
+        <f t="shared" si="42"/>
         <v>4.5353138653875025E-2</v>
       </c>
       <c r="L33" s="7">
-        <f>+L14/H14-1</f>
+        <f t="shared" si="42"/>
         <v>0.11312634835576207</v>
       </c>
       <c r="M33" s="7">
-        <f>+M14/I14-1</f>
+        <f t="shared" si="42"/>
         <v>0.19066880625250415</v>
       </c>
       <c r="N33" s="7">
-        <f>+N14/J14-1</f>
+        <f t="shared" si="42"/>
         <v>0.29127321004506457</v>
       </c>
       <c r="O33" s="7">
-        <f>+O14/K14-1</f>
-        <v>0.12784844953712704</v>
+        <f t="shared" si="42"/>
+        <v>0.30628929102289626</v>
       </c>
       <c r="P33" s="7">
-        <f>+P14/L14-1</f>
-        <v>0.11221268014712416</v>
+        <f t="shared" si="42"/>
+        <v>0.20005979174838684</v>
       </c>
       <c r="Q33" s="7">
-        <f>+Q14/M14-1</f>
-        <v>6.3824774872933698E-2</v>
+        <f t="shared" si="42"/>
+        <v>0.14766506539758506</v>
       </c>
       <c r="R33" s="7">
-        <f>+R14/N14-1</f>
-        <v>-1.1178529949966265E-2</v>
+        <f t="shared" si="42"/>
+        <v>6.6583534721734949E-2</v>
       </c>
       <c r="W33" s="7">
-        <f t="shared" ref="W33" si="26">+W14/V14-1</f>
+        <f t="shared" ref="W33" si="44">+W14/V14-1</f>
         <v>0.58850019926493369</v>
       </c>
       <c r="X33" s="7">
-        <f t="shared" ref="X33:Y33" si="27">+X14/W14-1</f>
+        <f t="shared" ref="X33:Y33" si="45">+X14/W14-1</f>
         <v>0.11345966755033721</v>
       </c>
       <c r="Y33" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="45"/>
         <v>0.12138846989165875</v>
       </c>
       <c r="Z33" s="7">
-        <f t="shared" ref="Z33" si="28">+Z14/Y14-1</f>
+        <f t="shared" ref="Z33" si="46">+Z14/Y14-1</f>
         <v>0.31999870512302464</v>
       </c>
       <c r="AA33" s="7">
-        <f t="shared" ref="AA33" si="29">+AA14/Z14-1</f>
+        <f t="shared" ref="AA33" si="47">+AA14/Z14-1</f>
         <v>0.48126392700242282</v>
       </c>
       <c r="AB33" s="7">
-        <f t="shared" ref="AB33:AC33" si="30">+AB14/AA14-1</f>
+        <f t="shared" ref="AB33:AC33" si="48">+AB14/AA14-1</f>
         <v>3.6389545113558741E-2</v>
       </c>
       <c r="AC33" s="7">
-        <f t="shared" si="30"/>
+        <f t="shared" si="48"/>
         <v>0.16458331267606896</v>
       </c>
       <c r="AD33" s="7">
-        <f t="shared" ref="AD33:AM33" si="31">+AD14/AC14-1</f>
-        <v>6.6472385485475849E-2</v>
+        <f t="shared" ref="AD33:AM33" si="49">+AD14/AC14-1</f>
+        <v>0.16915560738539503</v>
       </c>
       <c r="AE33" s="7">
-        <f t="shared" si="31"/>
-        <v>0.14349887600930589</v>
+        <f t="shared" si="49"/>
+        <v>7.3179052126631117E-2</v>
       </c>
       <c r="AF33" s="7">
-        <f t="shared" si="31"/>
-        <v>9.585152838427935E-2</v>
+        <f t="shared" si="49"/>
+        <v>9.5356371490280978E-2</v>
       </c>
       <c r="AG33" s="7">
-        <f t="shared" si="31"/>
-        <v>9.393305439330546E-2</v>
+        <f t="shared" si="49"/>
+        <v>9.3478260869565011E-2</v>
       </c>
       <c r="AH33" s="7">
-        <f t="shared" si="31"/>
-        <v>9.2168674698795083E-2</v>
+        <f t="shared" si="49"/>
+        <v>9.1749502982107378E-2</v>
       </c>
       <c r="AI33" s="7">
-        <f t="shared" si="31"/>
-        <v>9.0540540540540393E-2</v>
+        <f t="shared" si="49"/>
+        <v>9.0152963671128017E-2</v>
       </c>
       <c r="AJ33" s="7">
-        <f t="shared" si="31"/>
-        <v>8.9033457249070747E-2</v>
+        <f t="shared" si="49"/>
+        <v>8.8674033149171105E-2</v>
       </c>
       <c r="AK33" s="7">
-        <f t="shared" si="31"/>
-        <v>8.7634408602150549E-2</v>
+        <f t="shared" si="49"/>
+        <v>8.7300177619893393E-2</v>
       </c>
       <c r="AL33" s="7">
-        <f t="shared" si="31"/>
-        <v>8.6332179930795894E-2</v>
+        <f t="shared" si="49"/>
+        <v>8.6020583190394628E-2</v>
       </c>
       <c r="AM33" s="7">
-        <f t="shared" si="31"/>
-        <v>8.5117056856187423E-2</v>
+        <f t="shared" si="49"/>
+        <v>8.4825870646766388E-2</v>
       </c>
       <c r="AP33" s="7" t="s">
         <v>69</v>
       </c>
       <c r="AQ33" s="1">
         <f>+Main!G8</f>
-        <v>3749.4</v>
+        <v>3301.4659999999999</v>
       </c>
     </row>
     <row r="34" spans="2:43" s="7" customFormat="1">
@@ -3718,127 +3821,127 @@
         <v>19</v>
       </c>
       <c r="G34" s="7">
-        <f>+G15/C15-1</f>
+        <f t="shared" si="42"/>
         <v>0.30691089563371388</v>
       </c>
       <c r="H34" s="7">
-        <f>+H15/D15-1</f>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="I34" s="7">
-        <f>+I15/E15-1</f>
+        <f t="shared" si="42"/>
         <v>0.36948844840432904</v>
       </c>
       <c r="J34" s="7">
-        <f>+J15/F15-1</f>
+        <f t="shared" si="42"/>
         <v>0.34718732366793725</v>
       </c>
       <c r="K34" s="7">
-        <f>+K15/G15-1</f>
+        <f t="shared" si="42"/>
         <v>-9.8998382221548997E-4</v>
       </c>
       <c r="L34" s="7">
-        <f>+L15/H15-1</f>
+        <f t="shared" si="42"/>
         <v>-5.4201969360660684E-2</v>
       </c>
       <c r="M34" s="7">
-        <f>+M15/I15-1</f>
+        <f t="shared" si="42"/>
         <v>-0.12352328190295925</v>
       </c>
       <c r="N34" s="7">
-        <f>+N15/J15-1</f>
+        <f t="shared" si="42"/>
         <v>-0.17337445421939268</v>
       </c>
       <c r="O34" s="7">
-        <f>+O15/K15-1</f>
-        <v>0.12784844953712704</v>
+        <f t="shared" si="42"/>
+        <v>-1.1761939918086162E-2</v>
       </c>
       <c r="P34" s="7">
-        <f>+P15/L15-1</f>
-        <v>0.11221268014712438</v>
+        <f t="shared" si="42"/>
+        <v>0.20005979174838684</v>
       </c>
       <c r="Q34" s="7">
-        <f>+Q15/M15-1</f>
-        <v>6.3824774872933698E-2</v>
+        <f t="shared" si="42"/>
+        <v>0.14766506539758506</v>
       </c>
       <c r="R34" s="7">
-        <f>+R15/N15-1</f>
-        <v>-1.1178529949966265E-2</v>
+        <f t="shared" si="42"/>
+        <v>6.6583534721734949E-2</v>
       </c>
       <c r="W34" s="7">
-        <f t="shared" ref="W34" si="32">+W15/V15-1</f>
+        <f t="shared" ref="W34" si="50">+W15/V15-1</f>
         <v>7.3563612012456723</v>
       </c>
       <c r="X34" s="7">
-        <f t="shared" ref="X34:Y34" si="33">+X15/W15-1</f>
+        <f t="shared" ref="X34:Y34" si="51">+X15/W15-1</f>
         <v>-0.49690298091751517</v>
       </c>
       <c r="Y34" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="51"/>
         <v>0.14416752462169047</v>
       </c>
       <c r="Z34" s="7">
-        <f t="shared" ref="Z34" si="34">+Z15/Y15-1</f>
+        <f t="shared" ref="Z34" si="52">+Z15/Y15-1</f>
         <v>0.24680223970553761</v>
       </c>
       <c r="AA34" s="7">
-        <f t="shared" ref="AA34" si="35">+AA15/Z15-1</f>
+        <f t="shared" ref="AA34" si="53">+AA15/Z15-1</f>
         <v>0.54311290977077076</v>
       </c>
       <c r="AB34" s="7">
-        <f t="shared" ref="AB34:AC34" si="36">+AB15/AA15-1</f>
+        <f t="shared" ref="AB34:AC34" si="54">+AB15/AA15-1</f>
         <v>0.24118075128556771</v>
       </c>
       <c r="AC34" s="7">
-        <f t="shared" si="36"/>
+        <f t="shared" si="54"/>
         <v>-9.4292349985780732E-2</v>
       </c>
       <c r="AD34" s="7">
-        <f t="shared" ref="AD34:AM34" si="37">+AD15/AC15-1</f>
-        <v>7.2190034450207774E-2</v>
+        <f t="shared" ref="AD34:AM34" si="55">+AD15/AC15-1</f>
+        <v>0.10227439279278405</v>
       </c>
       <c r="AE34" s="7">
-        <f t="shared" si="37"/>
-        <v>0.14349887600930589</v>
+        <f t="shared" si="55"/>
+        <v>7.3179052126631339E-2</v>
       </c>
       <c r="AF34" s="7">
-        <f t="shared" si="37"/>
-        <v>9.585152838427935E-2</v>
+        <f t="shared" si="55"/>
+        <v>9.5356371490280756E-2</v>
       </c>
       <c r="AG34" s="7">
-        <f t="shared" si="37"/>
-        <v>9.393305439330546E-2</v>
+        <f t="shared" si="55"/>
+        <v>9.3478260869565233E-2</v>
       </c>
       <c r="AH34" s="7">
-        <f t="shared" si="37"/>
-        <v>9.2168674698795305E-2</v>
+        <f t="shared" si="55"/>
+        <v>9.1749502982107378E-2</v>
       </c>
       <c r="AI34" s="7">
-        <f t="shared" si="37"/>
-        <v>9.0540540540540615E-2</v>
+        <f t="shared" si="55"/>
+        <v>9.0152963671128239E-2</v>
       </c>
       <c r="AJ34" s="7">
-        <f t="shared" si="37"/>
-        <v>8.9033457249070524E-2</v>
+        <f t="shared" si="55"/>
+        <v>8.8674033149171327E-2</v>
       </c>
       <c r="AK34" s="7">
-        <f t="shared" si="37"/>
-        <v>8.7634408602150549E-2</v>
+        <f t="shared" si="55"/>
+        <v>8.7300177619893393E-2</v>
       </c>
       <c r="AL34" s="7">
-        <f t="shared" si="37"/>
-        <v>8.6332179930795894E-2</v>
+        <f t="shared" si="55"/>
+        <v>8.6020583190394628E-2</v>
       </c>
       <c r="AM34" s="7">
-        <f t="shared" si="37"/>
-        <v>8.5117056856187201E-2</v>
+        <f t="shared" si="55"/>
+        <v>8.4825870646766166E-2</v>
       </c>
       <c r="AP34" s="7" t="s">
         <v>70</v>
       </c>
       <c r="AQ34" s="1">
         <f>+AQ31+AQ32-AQ33</f>
-        <v>16494.586652799997</v>
+        <v>25003.058219900002</v>
       </c>
     </row>
     <row r="35" spans="2:43" s="7" customFormat="1">
@@ -3846,127 +3949,127 @@
         <v>41</v>
       </c>
       <c r="G35" s="7">
-        <f>+G16/C16-1</f>
+        <f t="shared" si="42"/>
         <v>0.60950454466816595</v>
       </c>
       <c r="H35" s="7">
-        <f>+H16/D16-1</f>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="I35" s="7">
-        <f>+I16/E16-1</f>
+        <f t="shared" si="42"/>
         <v>0.24277557625295376</v>
       </c>
       <c r="J35" s="7">
-        <f>+J16/F16-1</f>
+        <f t="shared" si="42"/>
         <v>0.20357381701926358</v>
       </c>
       <c r="K35" s="7">
-        <f>+K16/G16-1</f>
+        <f t="shared" si="42"/>
         <v>0.10975004754305751</v>
       </c>
       <c r="L35" s="7">
-        <f>+L16/H16-1</f>
+        <f t="shared" si="42"/>
         <v>-9.8842549474265851E-2</v>
       </c>
       <c r="M35" s="7">
-        <f>+M16/I16-1</f>
+        <f t="shared" si="42"/>
         <v>9.956128669507569E-2</v>
       </c>
       <c r="N35" s="7">
-        <f>+N16/J16-1</f>
+        <f t="shared" si="42"/>
         <v>-6.5522615619176716E-2</v>
       </c>
       <c r="O35" s="7">
-        <f>+O16/K16-1</f>
-        <v>0.12784844953712704</v>
+        <f t="shared" si="42"/>
+        <v>2.8316190632299287E-2</v>
       </c>
       <c r="P35" s="7">
-        <f>+P16/L16-1</f>
-        <v>0.11221268014712438</v>
+        <f t="shared" si="42"/>
+        <v>0.20005979174838684</v>
       </c>
       <c r="Q35" s="7">
-        <f>+Q16/M16-1</f>
-        <v>6.3824774872933476E-2</v>
+        <f t="shared" si="42"/>
+        <v>0.14766506539758484</v>
       </c>
       <c r="R35" s="7">
-        <f>+R16/N16-1</f>
-        <v>-1.1178529949966154E-2</v>
+        <f t="shared" si="42"/>
+        <v>6.6583534721734949E-2</v>
       </c>
       <c r="W35" s="7">
-        <f t="shared" ref="W35" si="38">+W16/V16-1</f>
+        <f t="shared" ref="W35" si="56">+W16/V16-1</f>
         <v>3.2019843854274717</v>
       </c>
       <c r="X35" s="7">
-        <f t="shared" ref="X35:Y35" si="39">+X16/W16-1</f>
+        <f t="shared" ref="X35:Y35" si="57">+X16/W16-1</f>
         <v>-0.23302685584715033</v>
       </c>
       <c r="Y35" s="7">
-        <f t="shared" si="39"/>
+        <f t="shared" si="57"/>
         <v>0.14413807556433755</v>
       </c>
       <c r="Z35" s="7">
-        <f t="shared" ref="Z35" si="40">+Z16/Y16-1</f>
+        <f t="shared" ref="Z35" si="58">+Z16/Y16-1</f>
         <v>0.21123075111535572</v>
       </c>
       <c r="AA35" s="7">
-        <f t="shared" ref="AA35" si="41">+AA16/Z16-1</f>
+        <f t="shared" ref="AA35" si="59">+AA16/Z16-1</f>
         <v>0.66420747909870603</v>
       </c>
       <c r="AB35" s="7">
-        <f t="shared" ref="AB35:AC35" si="42">+AB16/AA16-1</f>
+        <f t="shared" ref="AB35:AC35" si="60">+AB16/AA16-1</f>
         <v>0.2102218270168994</v>
       </c>
       <c r="AC35" s="7">
-        <f t="shared" si="42"/>
+        <f t="shared" si="60"/>
         <v>2.990848682363767E-3</v>
       </c>
       <c r="AD35" s="7">
-        <f t="shared" ref="AD35:AM35" si="43">+AD16/AC16-1</f>
-        <v>7.2805171855397477E-2</v>
+        <f t="shared" ref="AD35:AM35" si="61">+AD16/AC16-1</f>
+        <v>0.11228601312089936</v>
       </c>
       <c r="AE35" s="7">
-        <f t="shared" si="43"/>
-        <v>0.14349887600930589</v>
+        <f t="shared" si="61"/>
+        <v>7.3179052126631117E-2</v>
       </c>
       <c r="AF35" s="7">
-        <f t="shared" si="43"/>
-        <v>9.5851528384279572E-2</v>
+        <f t="shared" si="61"/>
+        <v>9.5356371490280978E-2</v>
       </c>
       <c r="AG35" s="7">
-        <f t="shared" si="43"/>
-        <v>9.3933054393305238E-2</v>
+        <f t="shared" si="61"/>
+        <v>9.3478260869565233E-2</v>
       </c>
       <c r="AH35" s="7">
-        <f t="shared" si="43"/>
-        <v>9.2168674698795305E-2</v>
+        <f t="shared" si="61"/>
+        <v>9.1749502982107378E-2</v>
       </c>
       <c r="AI35" s="7">
-        <f t="shared" si="43"/>
-        <v>9.0540540540540615E-2</v>
+        <f t="shared" si="61"/>
+        <v>9.0152963671128017E-2</v>
       </c>
       <c r="AJ35" s="7">
-        <f t="shared" si="43"/>
-        <v>8.9033457249070524E-2</v>
+        <f t="shared" si="61"/>
+        <v>8.8674033149171327E-2</v>
       </c>
       <c r="AK35" s="7">
-        <f t="shared" si="43"/>
-        <v>8.7634408602150549E-2</v>
+        <f t="shared" si="61"/>
+        <v>8.7300177619893393E-2</v>
       </c>
       <c r="AL35" s="7">
-        <f t="shared" si="43"/>
-        <v>8.6332179930795894E-2</v>
+        <f t="shared" si="61"/>
+        <v>8.6020583190394628E-2</v>
       </c>
       <c r="AM35" s="7">
-        <f t="shared" si="43"/>
-        <v>8.5117056856187201E-2</v>
+        <f t="shared" si="61"/>
+        <v>8.4825870646766388E-2</v>
       </c>
       <c r="AP35" s="7" t="s">
         <v>71</v>
       </c>
       <c r="AQ35" s="1">
         <f>+Main!G5</f>
-        <v>1650.6315199999999</v>
+        <v>1641.0389899999998</v>
       </c>
     </row>
     <row r="36" spans="2:43" s="7" customFormat="1">
@@ -3974,127 +4077,127 @@
         <v>20</v>
       </c>
       <c r="G36" s="7">
-        <f>+G17/C17-1</f>
+        <f t="shared" si="42"/>
         <v>0.33504819969948607</v>
       </c>
       <c r="H36" s="7">
-        <f>+H17/D17-1</f>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="I36" s="7">
-        <f>+I17/E17-1</f>
+        <f t="shared" si="42"/>
         <v>0.49688774782484679</v>
       </c>
       <c r="J36" s="7">
-        <f>+J17/F17-1</f>
+        <f t="shared" si="42"/>
         <v>0.16195908207243459</v>
       </c>
       <c r="K36" s="7">
-        <f>+K17/G17-1</f>
+        <f t="shared" si="42"/>
         <v>-0.11841617726068498</v>
       </c>
       <c r="L36" s="7">
-        <f>+L17/H17-1</f>
+        <f t="shared" si="42"/>
         <v>-0.12923340065285216</v>
       </c>
       <c r="M36" s="7">
-        <f>+M17/I17-1</f>
+        <f t="shared" si="42"/>
         <v>-0.15747407257772517</v>
       </c>
       <c r="N36" s="7">
-        <f>+N17/J17-1</f>
+        <f t="shared" si="42"/>
         <v>1.4287674446396892E-2</v>
       </c>
       <c r="O36" s="7">
-        <f>+O17/K17-1</f>
-        <v>0.12784844953712704</v>
+        <f t="shared" si="42"/>
+        <v>0.19502892177723141</v>
       </c>
       <c r="P36" s="7">
-        <f>+P17/L17-1</f>
-        <v>0.11221268014712438</v>
+        <f t="shared" si="42"/>
+        <v>0.20005979174838662</v>
       </c>
       <c r="Q36" s="7">
-        <f>+Q17/M17-1</f>
-        <v>6.3824774872933698E-2</v>
+        <f t="shared" si="42"/>
+        <v>0.14766506539758484</v>
       </c>
       <c r="R36" s="7">
-        <f>+R17/N17-1</f>
-        <v>-1.1178529949966265E-2</v>
+        <f t="shared" si="42"/>
+        <v>6.6583534721734949E-2</v>
       </c>
       <c r="W36" s="7">
-        <f t="shared" ref="W36" si="44">+W17/V17-1</f>
+        <f t="shared" ref="W36" si="62">+W17/V17-1</f>
         <v>8.297620489222572</v>
       </c>
       <c r="X36" s="7">
-        <f t="shared" ref="X36:Y36" si="45">+X17/W17-1</f>
+        <f t="shared" ref="X36:Y36" si="63">+X17/W17-1</f>
         <v>-0.68935689423318003</v>
       </c>
       <c r="Y36" s="7">
-        <f t="shared" si="45"/>
+        <f t="shared" si="63"/>
         <v>0.21779917907350188</v>
       </c>
       <c r="Z36" s="7">
-        <f t="shared" ref="Z36" si="46">+Z17/Y17-1</f>
+        <f t="shared" ref="Z36" si="64">+Z17/Y17-1</f>
         <v>-8.9088458420049754E-2</v>
       </c>
       <c r="AA36" s="7">
-        <f t="shared" ref="AA36" si="47">+AA17/Z17-1</f>
+        <f t="shared" ref="AA36" si="65">+AA17/Z17-1</f>
         <v>0.47496239351127434</v>
       </c>
       <c r="AB36" s="7">
-        <f t="shared" ref="AB36:AC36" si="48">+AB17/AA17-1</f>
+        <f t="shared" ref="AB36:AC36" si="66">+AB17/AA17-1</f>
         <v>0.22135639214500502</v>
       </c>
       <c r="AC36" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="66"/>
         <v>-0.10054077302743714</v>
       </c>
       <c r="AD36" s="7">
-        <f t="shared" ref="AD36:AM36" si="49">+AD17/AC17-1</f>
-        <v>7.0231037014712783E-2</v>
+        <f t="shared" ref="AD36:AM36" si="67">+AD17/AC17-1</f>
+        <v>0.14976197362686738</v>
       </c>
       <c r="AE36" s="7">
-        <f t="shared" si="49"/>
-        <v>0.14349887600930589</v>
+        <f t="shared" si="67"/>
+        <v>7.3179052126631117E-2</v>
       </c>
       <c r="AF36" s="7">
-        <f t="shared" si="49"/>
-        <v>9.585152838427935E-2</v>
+        <f t="shared" si="67"/>
+        <v>9.5356371490280978E-2</v>
       </c>
       <c r="AG36" s="7">
-        <f t="shared" si="49"/>
-        <v>9.3933054393305238E-2</v>
+        <f t="shared" si="67"/>
+        <v>9.3478260869565233E-2</v>
       </c>
       <c r="AH36" s="7">
-        <f t="shared" si="49"/>
-        <v>9.2168674698795305E-2</v>
+        <f t="shared" si="67"/>
+        <v>9.1749502982107378E-2</v>
       </c>
       <c r="AI36" s="7">
-        <f t="shared" si="49"/>
-        <v>9.0540540540540393E-2</v>
+        <f t="shared" si="67"/>
+        <v>9.0152963671128239E-2</v>
       </c>
       <c r="AJ36" s="7">
-        <f t="shared" si="49"/>
-        <v>8.9033457249070747E-2</v>
+        <f t="shared" si="67"/>
+        <v>8.8674033149171105E-2</v>
       </c>
       <c r="AK36" s="7">
-        <f t="shared" si="49"/>
-        <v>8.7634408602150549E-2</v>
+        <f t="shared" si="67"/>
+        <v>8.7300177619893393E-2</v>
       </c>
       <c r="AL36" s="7">
-        <f t="shared" si="49"/>
-        <v>8.6332179930795894E-2</v>
+        <f t="shared" si="67"/>
+        <v>8.6020583190394406E-2</v>
       </c>
       <c r="AM36" s="7">
-        <f t="shared" si="49"/>
-        <v>8.5117056856187201E-2</v>
+        <f t="shared" si="67"/>
+        <v>8.4825870646766388E-2</v>
       </c>
       <c r="AP36" s="7" t="s">
         <v>72</v>
       </c>
       <c r="AQ36" s="2">
         <f>+AQ34/AQ35</f>
-        <v>9.9928945091270265</v>
+        <v>15.236114664100702</v>
       </c>
     </row>
     <row r="37" spans="2:43">
@@ -4103,7 +4206,7 @@
       </c>
       <c r="AQ37" s="1">
         <f>+Main!G4</f>
-        <v>11.14</v>
+        <v>16.010000000000002</v>
       </c>
     </row>
     <row r="38" spans="2:43">
@@ -4112,7 +4215,7 @@
       </c>
       <c r="AQ38" s="11">
         <f>+AQ36/AQ37-1</f>
-        <v>-0.1029717675828522</v>
+        <v>-4.833762247965645E-2</v>
       </c>
     </row>
     <row r="39" spans="2:43">
@@ -4129,132 +4232,132 @@
         <v>0.53613510675897635</v>
       </c>
       <c r="D40" s="7">
-        <f t="shared" ref="D40:N40" si="50">+D14/D$13</f>
+        <f t="shared" ref="D40:N40" si="68">+D14/D$13</f>
         <v>0.4018123896736816</v>
       </c>
       <c r="E40" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="68"/>
         <v>0.41544266776333971</v>
       </c>
       <c r="F40" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="68"/>
         <v>0.34606378839419516</v>
       </c>
       <c r="G40" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="68"/>
         <v>0.39605373722508225</v>
       </c>
       <c r="H40" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="68"/>
         <v>0.4018123896736816</v>
       </c>
       <c r="I40" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="68"/>
         <v>0.41361712610635931</v>
       </c>
       <c r="J40" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="68"/>
         <v>0.37031471800020777</v>
       </c>
       <c r="K40" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="68"/>
         <v>0.44505607885026222</v>
       </c>
       <c r="L40" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="68"/>
         <v>0.4653820612942775</v>
       </c>
       <c r="M40" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="68"/>
         <v>0.46758868571899742</v>
       </c>
       <c r="N40" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="68"/>
         <v>0.45655618543334359</v>
       </c>
       <c r="O40" s="7">
-        <f t="shared" ref="O40:R40" si="51">+O14/O$13</f>
-        <v>0.44505607885026222</v>
+        <f t="shared" ref="O40:R40" si="69">+O14/O$13</f>
+        <v>0.48105288619679226</v>
       </c>
       <c r="P40" s="7">
-        <f t="shared" si="51"/>
+        <f t="shared" si="69"/>
         <v>0.4653820612942775</v>
       </c>
       <c r="Q40" s="7">
-        <f t="shared" si="51"/>
-        <v>0.46758868571899737</v>
+        <f t="shared" si="69"/>
+        <v>0.46758868571899748</v>
       </c>
       <c r="R40" s="7">
-        <f t="shared" si="51"/>
+        <f t="shared" si="69"/>
         <v>0.45655618543334359</v>
       </c>
       <c r="W40" s="7">
-        <f t="shared" ref="W40" si="52">+W14/W$13</f>
+        <f t="shared" ref="W40" si="70">+W14/W$13</f>
         <v>0.8697046726524913</v>
       </c>
       <c r="X40" s="7">
-        <f t="shared" ref="X40" si="53">+X14/X$13</f>
+        <f t="shared" ref="X40" si="71">+X14/X$13</f>
         <v>0.67674844931492006</v>
       </c>
       <c r="Y40" s="7">
-        <f t="shared" ref="Y40" si="54">+Y14/Y$13</f>
+        <f t="shared" ref="Y40" si="72">+Y14/Y$13</f>
         <v>0.52219192391406988</v>
       </c>
       <c r="Z40" s="7">
-        <f t="shared" ref="Z40" si="55">+Z14/Z$13</f>
+        <f t="shared" ref="Z40" si="73">+Z14/Z$13</f>
         <v>0.47175166937548724</v>
       </c>
       <c r="AA40" s="7">
-        <f t="shared" ref="AA40:AC40" si="56">+AA14/AA$13</f>
+        <f t="shared" ref="AA40:AC40" si="74">+AA14/AA$13</f>
         <v>0.4125445817785795</v>
       </c>
       <c r="AB40" s="7">
-        <f t="shared" si="56"/>
+        <f t="shared" si="74"/>
         <v>0.39448117245097447</v>
       </c>
       <c r="AC40" s="7">
-        <f t="shared" si="56"/>
+        <f t="shared" si="74"/>
         <v>0.45898050743413926</v>
       </c>
       <c r="AD40" s="7">
-        <f t="shared" ref="AD40:AM40" si="57">+AD14/AD$13</f>
-        <v>0.45891881489504294</v>
+        <f t="shared" ref="AD40:AM40" si="75">+AD14/AD$13</f>
+        <v>0.46706733733244055</v>
       </c>
       <c r="AE40" s="7">
-        <f t="shared" si="57"/>
-        <v>0.45891881489504294</v>
+        <f t="shared" si="75"/>
+        <v>0.46706733733244055</v>
       </c>
       <c r="AF40" s="7">
-        <f t="shared" si="57"/>
-        <v>0.45891881489504294</v>
+        <f t="shared" si="75"/>
+        <v>0.46706733733244055</v>
       </c>
       <c r="AG40" s="7">
-        <f t="shared" si="57"/>
-        <v>0.45891881489504294</v>
+        <f t="shared" si="75"/>
+        <v>0.46706733733244049</v>
       </c>
       <c r="AH40" s="7">
-        <f t="shared" si="57"/>
-        <v>0.45891881489504288</v>
+        <f t="shared" si="75"/>
+        <v>0.46706733733244049</v>
       </c>
       <c r="AI40" s="7">
-        <f t="shared" si="57"/>
-        <v>0.45891881489504288</v>
+        <f t="shared" si="75"/>
+        <v>0.46706733733244049</v>
       </c>
       <c r="AJ40" s="7">
-        <f t="shared" si="57"/>
-        <v>0.45891881489504288</v>
+        <f t="shared" si="75"/>
+        <v>0.46706733733244044</v>
       </c>
       <c r="AK40" s="7">
-        <f t="shared" si="57"/>
-        <v>0.45891881489504288</v>
+        <f t="shared" si="75"/>
+        <v>0.46706733733244044</v>
       </c>
       <c r="AL40" s="7">
-        <f t="shared" si="57"/>
-        <v>0.45891881489504294</v>
+        <f t="shared" si="75"/>
+        <v>0.46706733733244049</v>
       </c>
       <c r="AM40" s="7">
-        <f t="shared" si="57"/>
-        <v>0.45891881489504294</v>
+        <f t="shared" si="75"/>
+        <v>0.46706733733244049</v>
       </c>
     </row>
     <row r="41" spans="2:43">
@@ -4262,136 +4365,136 @@
         <v>19</v>
       </c>
       <c r="C41" s="7">
-        <f t="shared" ref="C41:N43" si="58">+C15/C$13</f>
+        <f t="shared" ref="C41:N43" si="76">+C15/C$13</f>
         <v>0.45294600719349676</v>
       </c>
       <c r="D41" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.45461599464942665</v>
       </c>
       <c r="E41" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.38597863548517947</v>
       </c>
       <c r="F41" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.33454042538437534</v>
       </c>
       <c r="G41" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.42867359161854357</v>
       </c>
       <c r="H41" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.45461599464942665</v>
       </c>
       <c r="I41" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.50001772301759184</v>
       </c>
       <c r="J41" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.45004712499086358</v>
       </c>
       <c r="K41" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.46035637987958833</v>
       </c>
       <c r="L41" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.44738865697140218</v>
       </c>
       <c r="M41" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.41610246426110453</v>
       </c>
       <c r="N41" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.35519916079416025</v>
       </c>
       <c r="O41" s="7">
-        <f t="shared" ref="O41:R41" si="59">+O15/O$13</f>
-        <v>0.46035637987958833</v>
+        <f t="shared" ref="O41:R41" si="77">+O15/O$13</f>
+        <v>0.37643887165176987</v>
       </c>
       <c r="P41" s="7">
-        <f t="shared" si="59"/>
+        <f t="shared" si="77"/>
         <v>0.44738865697140218</v>
       </c>
       <c r="Q41" s="7">
-        <f t="shared" si="59"/>
+        <f t="shared" si="77"/>
         <v>0.41610246426110453</v>
       </c>
       <c r="R41" s="7">
-        <f t="shared" si="59"/>
+        <f t="shared" si="77"/>
         <v>0.35519916079416025</v>
       </c>
       <c r="W41" s="7">
-        <f t="shared" ref="W41" si="60">+W15/W$13</f>
+        <f t="shared" ref="W41" si="78">+W15/W$13</f>
         <v>1.86055501612827</v>
       </c>
       <c r="X41" s="7">
-        <f t="shared" ref="X41" si="61">+X15/X$13</f>
+        <f t="shared" ref="X41" si="79">+X15/X$13</f>
         <v>0.65414682247218425</v>
       </c>
       <c r="Y41" s="7">
-        <f t="shared" ref="Y41" si="62">+Y15/Y$13</f>
+        <f t="shared" ref="Y41" si="80">+Y15/Y$13</f>
         <v>0.51500524035081785</v>
       </c>
       <c r="Z41" s="7">
-        <f t="shared" ref="Z41" si="63">+Z15/Z$13</f>
+        <f t="shared" ref="Z41" si="81">+Z15/Z$13</f>
         <v>0.43945965612739984</v>
       </c>
       <c r="AA41" s="7">
-        <f t="shared" ref="AA41:AC41" si="64">+AA15/AA$13</f>
+        <f t="shared" ref="AA41:AC41" si="82">+AA15/AA$13</f>
         <v>0.40035173177378652</v>
       </c>
       <c r="AB41" s="7">
-        <f t="shared" si="64"/>
+        <f t="shared" si="82"/>
         <v>0.45846808900860891</v>
       </c>
       <c r="AC41" s="7">
-        <f t="shared" si="64"/>
+        <f t="shared" si="82"/>
         <v>0.41485329827848416</v>
       </c>
       <c r="AD41" s="7">
-        <f t="shared" ref="AD41:AM41" si="65">+AD15/AD$13</f>
-        <v>0.41702137955692686</v>
+        <f t="shared" ref="AD41:AM41" si="83">+AD15/AD$13</f>
+        <v>0.39801295154478666</v>
       </c>
       <c r="AE41" s="7">
-        <f t="shared" si="65"/>
-        <v>0.41702137955692686</v>
+        <f t="shared" si="83"/>
+        <v>0.39801295154478666</v>
       </c>
       <c r="AF41" s="7">
-        <f t="shared" si="65"/>
-        <v>0.41702137955692686</v>
+        <f t="shared" si="83"/>
+        <v>0.39801295154478666</v>
       </c>
       <c r="AG41" s="7">
-        <f t="shared" si="65"/>
-        <v>0.41702137955692686</v>
+        <f t="shared" si="83"/>
+        <v>0.39801295154478666</v>
       </c>
       <c r="AH41" s="7">
-        <f t="shared" si="65"/>
-        <v>0.41702137955692686</v>
+        <f t="shared" si="83"/>
+        <v>0.39801295154478666</v>
       </c>
       <c r="AI41" s="7">
-        <f t="shared" si="65"/>
-        <v>0.41702137955692686</v>
+        <f t="shared" si="83"/>
+        <v>0.39801295154478666</v>
       </c>
       <c r="AJ41" s="7">
-        <f t="shared" si="65"/>
-        <v>0.41702137955692686</v>
+        <f t="shared" si="83"/>
+        <v>0.39801295154478666</v>
       </c>
       <c r="AK41" s="7">
-        <f t="shared" si="65"/>
-        <v>0.41702137955692686</v>
+        <f t="shared" si="83"/>
+        <v>0.39801295154478666</v>
       </c>
       <c r="AL41" s="7">
-        <f t="shared" si="65"/>
-        <v>0.41702137955692686</v>
+        <f t="shared" si="83"/>
+        <v>0.39801295154478672</v>
       </c>
       <c r="AM41" s="7">
-        <f t="shared" si="65"/>
-        <v>0.41702137955692686</v>
+        <f t="shared" si="83"/>
+        <v>0.39801295154478672</v>
       </c>
     </row>
     <row r="42" spans="2:43">
@@ -4399,136 +4502,136 @@
         <v>41</v>
       </c>
       <c r="C42" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.19528212644753531</v>
       </c>
       <c r="D42" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.28028758431158629</v>
       </c>
       <c r="E42" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.20377696443275745</v>
       </c>
       <c r="F42" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.18894432095293498</v>
       </c>
       <c r="G42" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.22760878381748084</v>
       </c>
       <c r="H42" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.28028758431158629</v>
       </c>
       <c r="I42" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.2395584841857514</v>
       </c>
       <c r="J42" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.22708475189173177</v>
       </c>
       <c r="K42" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.27152622677542565</v>
       </c>
       <c r="L42" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.26281272566684988</v>
       </c>
       <c r="M42" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.25009528408961834</v>
       </c>
       <c r="N42" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.2026104708265046</v>
       </c>
       <c r="O42" s="7">
-        <f t="shared" ref="O42:R42" si="66">+O16/O$13</f>
-        <v>0.27152622677542565</v>
+        <f t="shared" ref="O42:R42" si="84">+O16/O$13</f>
+        <v>0.23103468190191778</v>
       </c>
       <c r="P42" s="7">
-        <f t="shared" si="66"/>
+        <f t="shared" si="84"/>
         <v>0.26281272566684988</v>
       </c>
       <c r="Q42" s="7">
-        <f t="shared" si="66"/>
+        <f t="shared" si="84"/>
         <v>0.25009528408961834</v>
       </c>
       <c r="R42" s="7">
-        <f t="shared" si="66"/>
-        <v>0.20261047082650463</v>
+        <f t="shared" si="84"/>
+        <v>0.2026104708265046</v>
       </c>
       <c r="W42" s="7">
-        <f t="shared" ref="W42" si="67">+W16/W$13</f>
+        <f t="shared" ref="W42" si="85">+W16/W$13</f>
         <v>0.63349976786443774</v>
       </c>
       <c r="X42" s="7">
-        <f t="shared" ref="X42" si="68">+X16/X$13</f>
+        <f t="shared" ref="X42" si="86">+X16/X$13</f>
         <v>0.33955301640227509</v>
       </c>
       <c r="Y42" s="7">
-        <f t="shared" ref="Y42" si="69">+Y16/Y$13</f>
+        <f t="shared" ref="Y42" si="87">+Y16/Y$13</f>
         <v>0.26732084587073179</v>
       </c>
       <c r="Z42" s="7">
-        <f t="shared" ref="Z42" si="70">+Z16/Z$13</f>
+        <f t="shared" ref="Z42" si="88">+Z16/Z$13</f>
         <v>0.22159987170004616</v>
       </c>
       <c r="AA42" s="7">
-        <f t="shared" ref="AA42:AC42" si="71">+AA16/AA$13</f>
+        <f t="shared" ref="AA42:AC42" si="89">+AA16/AA$13</f>
         <v>0.21772182665940309</v>
       </c>
       <c r="AB42" s="7">
-        <f t="shared" si="71"/>
+        <f t="shared" si="89"/>
         <v>0.24310803901129263</v>
       </c>
       <c r="AC42" s="7">
-        <f t="shared" si="71"/>
+        <f t="shared" si="89"/>
         <v>0.24360920211501447</v>
       </c>
       <c r="AD42" s="7">
-        <f t="shared" ref="AD42:AM42" si="72">+AD16/AD$13</f>
-        <v>0.24502283184750265</v>
+        <f t="shared" ref="AD42:AM42" si="90">+AD16/AD$13</f>
+        <v>0.23584306172710212</v>
       </c>
       <c r="AE42" s="7">
-        <f t="shared" si="72"/>
-        <v>0.24502283184750265</v>
+        <f t="shared" si="90"/>
+        <v>0.23584306172710212</v>
       </c>
       <c r="AF42" s="7">
-        <f t="shared" si="72"/>
-        <v>0.24502283184750265</v>
+        <f t="shared" si="90"/>
+        <v>0.23584306172710215</v>
       </c>
       <c r="AG42" s="7">
-        <f t="shared" si="72"/>
-        <v>0.24502283184750265</v>
+        <f t="shared" si="90"/>
+        <v>0.23584306172710215</v>
       </c>
       <c r="AH42" s="7">
-        <f t="shared" si="72"/>
-        <v>0.24502283184750265</v>
+        <f t="shared" si="90"/>
+        <v>0.23584306172710215</v>
       </c>
       <c r="AI42" s="7">
-        <f t="shared" si="72"/>
-        <v>0.24502283184750265</v>
+        <f t="shared" si="90"/>
+        <v>0.23584306172710215</v>
       </c>
       <c r="AJ42" s="7">
-        <f t="shared" si="72"/>
-        <v>0.24502283184750262</v>
+        <f t="shared" si="90"/>
+        <v>0.23584306172710218</v>
       </c>
       <c r="AK42" s="7">
-        <f t="shared" si="72"/>
-        <v>0.24502283184750265</v>
+        <f t="shared" si="90"/>
+        <v>0.23584306172710218</v>
       </c>
       <c r="AL42" s="7">
-        <f t="shared" si="72"/>
-        <v>0.24502283184750265</v>
+        <f t="shared" si="90"/>
+        <v>0.23584306172710218</v>
       </c>
       <c r="AM42" s="7">
-        <f t="shared" si="72"/>
-        <v>0.24502283184750262</v>
+        <f t="shared" si="90"/>
+        <v>0.23584306172710218</v>
       </c>
     </row>
     <row r="43" spans="2:43">
@@ -4536,136 +4639,136 @@
         <v>20</v>
       </c>
       <c r="C43" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.21014340214973287</v>
       </c>
       <c r="D43" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.22419568119440925</v>
       </c>
       <c r="E43" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.16419649807816794</v>
       </c>
       <c r="F43" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.14981142397053668</v>
       </c>
       <c r="G43" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.20316412399421485</v>
       </c>
       <c r="H43" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.22419568119440925</v>
       </c>
       <c r="I43" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.23249674782627189</v>
       </c>
       <c r="J43" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.17382697242130127</v>
       </c>
       <c r="K43" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.19253435133035543</v>
       </c>
       <c r="L43" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.20312849768982708</v>
       </c>
       <c r="M43" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.18598360524706134</v>
       </c>
       <c r="N43" s="7">
-        <f t="shared" si="58"/>
+        <f t="shared" si="76"/>
         <v>0.16833849144228955</v>
       </c>
       <c r="O43" s="7">
-        <f t="shared" ref="O43:R43" si="73">+O17/O$13</f>
-        <v>0.19253435133035543</v>
+        <f t="shared" ref="O43:R43" si="91">+O17/O$13</f>
+        <v>0.19038177126533659</v>
       </c>
       <c r="P43" s="7">
-        <f t="shared" si="73"/>
+        <f t="shared" si="91"/>
         <v>0.20312849768982708</v>
       </c>
       <c r="Q43" s="7">
-        <f t="shared" si="73"/>
+        <f t="shared" si="91"/>
         <v>0.18598360524706134</v>
       </c>
       <c r="R43" s="7">
-        <f t="shared" si="73"/>
+        <f t="shared" si="91"/>
         <v>0.16833849144228955</v>
       </c>
       <c r="W43" s="7">
-        <f t="shared" ref="W43" si="74">+W17/W$13</f>
+        <f t="shared" ref="W43" si="92">+W17/W$13</f>
         <v>1.8614423437085204</v>
       </c>
       <c r="X43" s="7">
-        <f t="shared" ref="X43" si="75">+X17/X$13</f>
+        <f t="shared" ref="X43" si="93">+X17/X$13</f>
         <v>0.40410319489413327</v>
       </c>
       <c r="Y43" s="7">
-        <f t="shared" ref="Y43" si="76">+Y17/Y$13</f>
+        <f t="shared" ref="Y43" si="94">+Y17/Y$13</f>
         <v>0.3386216769822108</v>
       </c>
       <c r="Z43" s="7">
-        <f t="shared" ref="Z43" si="77">+Z17/Z$13</f>
+        <f t="shared" ref="Z43" si="95">+Z17/Z$13</f>
         <v>0.21110608443381659</v>
       </c>
       <c r="AA43" s="7">
-        <f t="shared" ref="AA43:AC43" si="78">+AA17/AA$13</f>
+        <f t="shared" ref="AA43:AC43" si="96">+AA17/AA$13</f>
         <v>0.18382589677588626</v>
       </c>
       <c r="AB43" s="7">
-        <f t="shared" si="78"/>
+        <f t="shared" si="96"/>
         <v>0.20714834717451489</v>
       </c>
       <c r="AC43" s="7">
-        <f t="shared" si="78"/>
+        <f t="shared" si="96"/>
         <v>0.18614884778169893</v>
       </c>
       <c r="AD43" s="7">
-        <f t="shared" ref="AD43:AM43" si="79">+AD17/AD$13</f>
-        <v>0.18677979779409301</v>
+        <f t="shared" ref="AD43:AM43" si="97">+AD17/AD$13</f>
+        <v>0.18628643527562494</v>
       </c>
       <c r="AE43" s="7">
-        <f t="shared" si="79"/>
-        <v>0.18677979779409298</v>
+        <f t="shared" si="97"/>
+        <v>0.18628643527562494</v>
       </c>
       <c r="AF43" s="7">
-        <f t="shared" si="79"/>
-        <v>0.18677979779409296</v>
+        <f t="shared" si="97"/>
+        <v>0.18628643527562494</v>
       </c>
       <c r="AG43" s="7">
-        <f t="shared" si="79"/>
-        <v>0.18677979779409296</v>
+        <f t="shared" si="97"/>
+        <v>0.18628643527562494</v>
       </c>
       <c r="AH43" s="7">
-        <f t="shared" si="79"/>
-        <v>0.18677979779409293</v>
+        <f t="shared" si="97"/>
+        <v>0.18628643527562494</v>
       </c>
       <c r="AI43" s="7">
-        <f t="shared" si="79"/>
-        <v>0.18677979779409293</v>
+        <f t="shared" si="97"/>
+        <v>0.18628643527562494</v>
       </c>
       <c r="AJ43" s="7">
-        <f t="shared" si="79"/>
-        <v>0.18677979779409293</v>
+        <f t="shared" si="97"/>
+        <v>0.18628643527562494</v>
       </c>
       <c r="AK43" s="7">
-        <f t="shared" si="79"/>
-        <v>0.18677979779409293</v>
+        <f t="shared" si="97"/>
+        <v>0.18628643527562494</v>
       </c>
       <c r="AL43" s="7">
-        <f t="shared" si="79"/>
-        <v>0.18677979779409293</v>
+        <f t="shared" si="97"/>
+        <v>0.18628643527562494</v>
       </c>
       <c r="AM43" s="7">
-        <f t="shared" si="79"/>
-        <v>0.18677979779409293</v>
+        <f t="shared" si="97"/>
+        <v>0.18628643527562494</v>
       </c>
     </row>
     <row r="46" spans="2:43" s="9" customFormat="1">
@@ -4673,68 +4776,72 @@
         <v>62</v>
       </c>
       <c r="J46" s="9">
-        <f t="shared" ref="J46:M46" si="80">+SUM(J47:J48)-J61</f>
+        <f t="shared" ref="J46:M46" si="98">+SUM(J47:J48)-J61</f>
         <v>196.60400000000027</v>
       </c>
       <c r="K46" s="9">
-        <f t="shared" si="80"/>
+        <f t="shared" si="98"/>
         <v>3204.5349999999999</v>
       </c>
       <c r="L46" s="9">
-        <f t="shared" si="80"/>
+        <f t="shared" si="98"/>
         <v>-56.678000000000338</v>
       </c>
       <c r="M46" s="9">
-        <f t="shared" si="80"/>
+        <f t="shared" si="98"/>
         <v>-134.17900000000009</v>
       </c>
       <c r="N46" s="9">
         <f>+SUM(N47:N48)-N61</f>
         <v>-205.32000000000016</v>
       </c>
+      <c r="O46" s="9">
+        <f>+SUM(O47:O48)-O61</f>
+        <v>-390.45099999999957</v>
+      </c>
       <c r="AC46" s="9">
         <f>+N46</f>
         <v>-205.32000000000016</v>
       </c>
       <c r="AD46" s="9">
         <f>+AC46+AD25</f>
-        <v>-1722.2952940859157</v>
+        <v>-1722.5156460247795</v>
       </c>
       <c r="AE46" s="9">
-        <f t="shared" ref="AE46:AM46" si="81">+AD46+AE25</f>
-        <v>-3521.204820316982</v>
+        <f t="shared" ref="AE46:AM46" si="99">+AD46+AE25</f>
+        <v>-3436.7740225814878</v>
       </c>
       <c r="AF46" s="9">
-        <f t="shared" si="81"/>
-        <v>-5469.8165986249696</v>
+        <f t="shared" si="99"/>
+        <v>-5292.6477973453457</v>
       </c>
       <c r="AG46" s="9">
-        <f t="shared" si="81"/>
-        <v>-7579.0267780627182</v>
+        <f t="shared" si="99"/>
+        <v>-7300.4308682375013</v>
       </c>
       <c r="AH46" s="9">
-        <f t="shared" si="81"/>
-        <v>-9860.4425784047871</v>
+        <f t="shared" si="99"/>
+        <v>-9471.0882072517725</v>
       </c>
       <c r="AI46" s="9">
-        <f t="shared" si="81"/>
-        <v>-12326.426200305857</v>
+        <f t="shared" si="99"/>
+        <v>-11816.297276883783</v>
       </c>
       <c r="AJ46" s="9">
-        <f t="shared" si="81"/>
-        <v>-14990.141348357778</v>
+        <f t="shared" si="99"/>
+        <v>-14348.491910069986</v>
       </c>
       <c r="AK46" s="9">
-        <f t="shared" si="81"/>
-        <v>-17865.602518564174</v>
+        <f t="shared" si="99"/>
+        <v>-17080.908796451069</v>
       </c>
       <c r="AL46" s="9">
-        <f t="shared" si="81"/>
-        <v>-20967.727210371158</v>
+        <f t="shared" si="99"/>
+        <v>-20027.636725896886</v>
       </c>
       <c r="AM46" s="9">
-        <f t="shared" si="81"/>
-        <v>-24312.39123249544</v>
+        <f t="shared" si="99"/>
+        <v>-23203.668748807875</v>
       </c>
     </row>
     <row r="47" spans="2:43">
@@ -4756,6 +4863,9 @@
       <c r="N47" s="1">
         <v>1780.4</v>
       </c>
+      <c r="O47" s="1">
+        <v>1060.393</v>
+      </c>
     </row>
     <row r="48" spans="2:43">
       <c r="B48" s="1" t="s">
@@ -4776,8 +4886,11 @@
       <c r="N48" s="1">
         <v>1763.68</v>
       </c>
-    </row>
-    <row r="49" spans="2:14">
+      <c r="O48" s="1">
+        <v>1850.6220000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15">
       <c r="B49" s="1" t="s">
         <v>48</v>
       </c>
@@ -4796,8 +4909,11 @@
       <c r="N49" s="1">
         <v>1278.1759999999999</v>
       </c>
-    </row>
-    <row r="50" spans="2:14">
+      <c r="O49" s="1">
+        <v>1108.357</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15">
       <c r="B50" s="1" t="s">
         <v>49</v>
       </c>
@@ -4816,8 +4932,11 @@
       <c r="N50" s="1">
         <v>153.58699999999999</v>
       </c>
-    </row>
-    <row r="51" spans="2:14">
+      <c r="O50" s="1">
+        <v>167.38499999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="2:15">
       <c r="B51" s="1" t="s">
         <v>50</v>
       </c>
@@ -4836,8 +4955,11 @@
       <c r="N51" s="1">
         <v>410.32600000000002</v>
       </c>
-    </row>
-    <row r="52" spans="2:14">
+      <c r="O51" s="1">
+        <v>426.363</v>
+      </c>
+    </row>
+    <row r="52" spans="2:15">
       <c r="B52" s="1" t="s">
         <v>51</v>
       </c>
@@ -4856,8 +4978,11 @@
       <c r="N52" s="1">
         <v>516.86199999999997</v>
       </c>
-    </row>
-    <row r="53" spans="2:14">
+      <c r="O52" s="1">
+        <v>511.11700000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15">
       <c r="B53" s="1" t="s">
         <v>52</v>
       </c>
@@ -4876,8 +5001,11 @@
       <c r="N53" s="1">
         <v>146.303</v>
       </c>
-    </row>
-    <row r="54" spans="2:14">
+      <c r="O53" s="1">
+        <v>127.658</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15">
       <c r="B54" s="1" t="s">
         <v>53</v>
       </c>
@@ -4896,8 +5024,11 @@
       <c r="N54" s="1">
         <v>1691.827</v>
       </c>
-    </row>
-    <row r="55" spans="2:14">
+      <c r="O54" s="1">
+        <v>1691.5239999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15">
       <c r="B55" s="1" t="s">
         <v>54</v>
       </c>
@@ -4936,29 +5067,32 @@
       <c r="N55" s="1">
         <v>226.59700000000001</v>
       </c>
-    </row>
-    <row r="56" spans="2:14">
+      <c r="O55" s="1">
+        <v>223.982</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15">
       <c r="B56" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E56" s="1">
-        <f t="shared" ref="E56:L56" si="82">+SUM(E47:E55)</f>
+        <f t="shared" ref="E56:L56" si="100">+SUM(E47:E55)</f>
         <v>0</v>
       </c>
       <c r="F56" s="1">
-        <f t="shared" si="82"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="G56" s="1">
-        <f t="shared" si="82"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="H56" s="1">
-        <f t="shared" si="82"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="I56" s="1">
-        <f t="shared" si="82"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="J56" s="1">
@@ -4966,11 +5100,11 @@
         <v>8029.5379999999996</v>
       </c>
       <c r="K56" s="1">
-        <f t="shared" si="82"/>
+        <f t="shared" si="100"/>
         <v>7888.3899999999994</v>
       </c>
       <c r="L56" s="1">
-        <f t="shared" si="82"/>
+        <f t="shared" si="100"/>
         <v>7666.223</v>
       </c>
       <c r="M56" s="1">
@@ -4981,8 +5115,12 @@
         <f>+SUM(N47:N55)</f>
         <v>7967.7579999999989</v>
       </c>
-    </row>
-    <row r="58" spans="2:14">
+      <c r="O56" s="1">
+        <f>+SUM(O47:O55)</f>
+        <v>7167.4010000000017</v>
+      </c>
+    </row>
+    <row r="58" spans="2:15">
       <c r="B58" s="1" t="s">
         <v>57</v>
       </c>
@@ -5001,8 +5139,11 @@
       <c r="N58" s="1">
         <v>278.96100000000001</v>
       </c>
-    </row>
-    <row r="59" spans="2:14">
+      <c r="O58" s="1">
+        <v>246.21700000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="2:15">
       <c r="B59" s="1" t="s">
         <v>58</v>
       </c>
@@ -5021,8 +5162,11 @@
       <c r="N59" s="1">
         <v>49.320999999999998</v>
       </c>
-    </row>
-    <row r="60" spans="2:14">
+      <c r="O59" s="1">
+        <v>36.649000000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="2:15">
       <c r="B60" s="1" t="s">
         <v>59</v>
       </c>
@@ -5041,8 +5185,11 @@
       <c r="N60" s="1">
         <v>805.83600000000001</v>
       </c>
-    </row>
-    <row r="61" spans="2:14">
+      <c r="O60" s="1">
+        <v>829.57899999999995</v>
+      </c>
+    </row>
+    <row r="61" spans="2:15">
       <c r="B61" s="1" t="s">
         <v>60</v>
       </c>
@@ -5061,8 +5208,11 @@
       <c r="N61" s="1">
         <v>3749.4</v>
       </c>
-    </row>
-    <row r="62" spans="2:14">
+      <c r="O61" s="1">
+        <v>3301.4659999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="2:15">
       <c r="B62" s="1" t="s">
         <v>58</v>
       </c>
@@ -5081,8 +5231,11 @@
       <c r="N62" s="1">
         <v>546.279</v>
       </c>
-    </row>
-    <row r="63" spans="2:14">
+      <c r="O62" s="1">
+        <v>553.74099999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="2:15">
       <c r="B63" s="1" t="s">
         <v>61</v>
       </c>
@@ -5101,8 +5254,11 @@
       <c r="N63" s="1">
         <v>123.849</v>
       </c>
-    </row>
-    <row r="64" spans="2:14">
+      <c r="O63" s="1">
+        <v>68.400999999999996</v>
+      </c>
+    </row>
+    <row r="64" spans="2:15">
       <c r="B64" s="1" t="s">
         <v>55</v>
       </c>
@@ -5121,53 +5277,60 @@
       <c r="N64" s="1">
         <v>2414.1120000000001</v>
       </c>
-    </row>
-    <row r="65" spans="2:14">
+      <c r="O64" s="1">
+        <v>2131.348</v>
+      </c>
+    </row>
+    <row r="65" spans="2:15">
       <c r="B65" s="1" t="s">
         <v>56</v>
       </c>
       <c r="E65" s="1">
-        <f t="shared" ref="E65:M65" si="83">SUM(E58:E64)</f>
+        <f t="shared" ref="E65:M65" si="101">SUM(E58:E64)</f>
         <v>0</v>
       </c>
       <c r="F65" s="1">
-        <f t="shared" si="83"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="G65" s="1">
-        <f t="shared" si="83"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="H65" s="1">
-        <f t="shared" si="83"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="I65" s="1">
-        <f t="shared" si="83"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="J65" s="1">
-        <f t="shared" si="83"/>
+        <f t="shared" si="101"/>
         <v>8029.5380000000005</v>
       </c>
       <c r="K65" s="1">
-        <f t="shared" si="83"/>
+        <f t="shared" si="101"/>
         <v>5360.7370000000001</v>
       </c>
       <c r="L65" s="1">
-        <f t="shared" si="83"/>
+        <f t="shared" si="101"/>
         <v>7666.223</v>
       </c>
       <c r="M65" s="1">
-        <f t="shared" si="83"/>
+        <f t="shared" si="101"/>
         <v>7722.9050000000007</v>
       </c>
       <c r="N65" s="1">
         <f>SUM(N58:N64)</f>
         <v>7967.7580000000007</v>
       </c>
-    </row>
-    <row r="71" spans="2:14">
+      <c r="O65" s="1">
+        <f>SUM(O58:O64)</f>
+        <v>7167.4009999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="2:15">
       <c r="B71" s="1" t="s">
         <v>63</v>
       </c>
@@ -5195,8 +5358,11 @@
       <c r="N71" s="1">
         <v>164.57400000000001</v>
       </c>
-    </row>
-    <row r="72" spans="2:14">
+      <c r="O71" s="1">
+        <v>88.352000000000004</v>
+      </c>
+    </row>
+    <row r="72" spans="2:15">
       <c r="B72" s="1" t="s">
         <v>64</v>
       </c>
@@ -5224,41 +5390,45 @@
       <c r="N72" s="1">
         <v>-53.719000000000001</v>
       </c>
-    </row>
-    <row r="73" spans="2:14" s="9" customFormat="1">
+      <c r="O72" s="1">
+        <f>+-50.448</f>
+        <v>-50.448</v>
+      </c>
+    </row>
+    <row r="73" spans="2:15" s="9" customFormat="1">
       <c r="B73" s="9" t="s">
         <v>65</v>
       </c>
       <c r="E73" s="9">
-        <f t="shared" ref="E73:L73" si="84">SUM(E71:E72)</f>
+        <f t="shared" ref="E73:L73" si="102">SUM(E71:E72)</f>
         <v>0</v>
       </c>
       <c r="F73" s="9">
-        <f t="shared" si="84"/>
+        <f t="shared" si="102"/>
         <v>0</v>
       </c>
       <c r="G73" s="9">
-        <f t="shared" si="84"/>
+        <f t="shared" si="102"/>
         <v>106.28400000000001</v>
       </c>
       <c r="H73" s="9">
-        <f t="shared" si="84"/>
+        <f t="shared" si="102"/>
         <v>-147.45099999999999</v>
       </c>
       <c r="I73" s="9">
-        <f t="shared" si="84"/>
+        <f t="shared" si="102"/>
         <v>18.109000000000002</v>
       </c>
       <c r="J73" s="9">
-        <f t="shared" si="84"/>
+        <f t="shared" si="102"/>
         <v>78.366</v>
       </c>
       <c r="K73" s="9">
-        <f t="shared" si="84"/>
+        <f t="shared" si="102"/>
         <v>103.47200000000001</v>
       </c>
       <c r="L73" s="9">
-        <f t="shared" si="84"/>
+        <f t="shared" si="102"/>
         <v>-118.879</v>
       </c>
       <c r="M73" s="9">
@@ -5268,6 +5438,68 @@
       <c r="N73" s="9">
         <f>SUM(N71:N72)</f>
         <v>110.85500000000002</v>
+      </c>
+      <c r="O73" s="9">
+        <f>SUM(O71:O72)</f>
+        <v>37.904000000000003</v>
+      </c>
+    </row>
+    <row r="75" spans="2:15">
+      <c r="B75" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J75" s="1">
+        <f t="shared" ref="J75:N75" si="103">+SUM(G73:J73)</f>
+        <v>55.308000000000014</v>
+      </c>
+      <c r="K75" s="1">
+        <f t="shared" si="103"/>
+        <v>52.496000000000024</v>
+      </c>
+      <c r="L75" s="1">
+        <f t="shared" si="103"/>
+        <v>81.067999999999998</v>
+      </c>
+      <c r="M75" s="1">
+        <f t="shared" si="103"/>
+        <v>2.3050000000000139</v>
+      </c>
+      <c r="N75" s="1">
+        <f t="shared" si="103"/>
+        <v>34.794000000000011</v>
+      </c>
+      <c r="O75" s="1">
+        <f>+SUM(L73:O73)</f>
+        <v>-30.773999999999994</v>
+      </c>
+    </row>
+    <row r="76" spans="2:15">
+      <c r="B76" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J76" s="1">
+        <f t="shared" ref="J76:N76" si="104">+SUM(G25:J25)</f>
+        <v>-1145.3989999999994</v>
+      </c>
+      <c r="K76" s="1">
+        <f t="shared" si="104"/>
+        <v>-1114.4489999999996</v>
+      </c>
+      <c r="L76" s="1">
+        <f t="shared" si="104"/>
+        <v>-1069.6899999999998</v>
+      </c>
+      <c r="M76" s="1">
+        <f t="shared" si="104"/>
+        <v>-1078.444</v>
+      </c>
+      <c r="N76" s="1">
+        <f t="shared" si="104"/>
+        <v>-1322.4850000000001</v>
+      </c>
+      <c r="O76" s="1">
+        <f>+SUM(L25:O25)</f>
+        <v>-1298.9010000000001</v>
       </c>
     </row>
   </sheetData>
@@ -5276,9 +5508,11 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="K19:K27 I20:I22 I24 E19:E27 I26 G19:I19 G23:I23 G20:G22 G25:I25 G24 G27:I27 G26 C18:N18 Z31:AC31 AA13:AC17 AA19:AC24 AA27:AC27 T18:AC18 F46:I46 Z28:AC28 AD23:AD27 J45:N46" formulaRange="1"/>
-    <ignoredError sqref="AA26:AC26 AA25:AC25" formula="1" formulaRange="1"/>
+    <ignoredError sqref="K19:K27 I20:I22 I24 E19:E27 I26 G19:I19 G23:I23 G20:G22 G25:I25 G24 G27:I27 G26 C18:N18 Z31:AC31 AA13:AC17 AA19:AC24 AA27:AC27 T18:AC18 F46:I46 Z28:AC28 J45:N46" formulaRange="1"/>
+    <ignoredError sqref="AA26:AC26 AA25:AC25 AD23:AD27" formula="1" formulaRange="1"/>
+    <ignoredError sqref="AD20:AD22 AD28:AD31" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>